<commit_message>
till the demo given on 17th
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -614,7 +614,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -758,7 +758,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2054,7 +2054,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -3422,7 +3422,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -3782,7 +3782,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -3854,7 +3854,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -4502,7 +4502,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
@@ -4790,7 +4790,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -4898,7 +4898,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -5366,7 +5366,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
@@ -5654,7 +5654,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
@@ -5690,7 +5690,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -5798,7 +5798,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -6122,7 +6122,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
@@ -6266,7 +6266,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
@@ -6482,7 +6482,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -6590,7 +6590,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -6662,7 +6662,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
@@ -6734,7 +6734,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -7094,7 +7094,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -7202,7 +7202,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
@@ -7562,7 +7562,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
@@ -7598,7 +7598,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -7634,7 +7634,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
@@ -7886,7 +7886,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
@@ -7994,7 +7994,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -8138,7 +8138,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
@@ -8174,7 +8174,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
@@ -8246,7 +8246,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -8318,7 +8318,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
@@ -8534,7 +8534,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -8570,7 +8570,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -8966,7 +8966,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
@@ -9002,7 +9002,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
@@ -9074,7 +9074,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -9110,7 +9110,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -9254,7 +9254,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
@@ -9362,7 +9362,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
@@ -9398,7 +9398,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -9506,7 +9506,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
@@ -9578,7 +9578,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
@@ -9794,7 +9794,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
@@ -9830,7 +9830,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
@@ -9866,7 +9866,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
@@ -9902,7 +9902,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
@@ -10010,7 +10010,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -10262,7 +10262,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H273" t="inlineStr">
@@ -10586,7 +10586,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H282" t="inlineStr">
@@ -10622,7 +10622,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H283" t="inlineStr">
@@ -10658,7 +10658,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H284" t="inlineStr">
@@ -10766,7 +10766,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H287" t="inlineStr">
@@ -10802,7 +10802,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H288" t="inlineStr">
@@ -10982,7 +10982,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
@@ -11054,7 +11054,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
@@ -11126,7 +11126,7 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H297" t="inlineStr">
@@ -11270,7 +11270,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -11306,7 +11306,7 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H302" t="inlineStr">
@@ -11342,7 +11342,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -11450,7 +11450,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -11738,7 +11738,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H314" t="inlineStr">
@@ -11810,7 +11810,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -11918,7 +11918,7 @@
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H319" t="inlineStr">
@@ -11954,7 +11954,7 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H320" t="inlineStr">
@@ -12170,7 +12170,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -12206,7 +12206,7 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H327" t="inlineStr">
@@ -12278,7 +12278,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H329" t="inlineStr">
@@ -12458,7 +12458,7 @@
       </c>
       <c r="G334" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H334" t="inlineStr">
@@ -12782,7 +12782,7 @@
       </c>
       <c r="G343" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H343" t="inlineStr">
@@ -12818,7 +12818,7 @@
       </c>
       <c r="G344" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H344" t="inlineStr">
@@ -12890,7 +12890,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H346" t="inlineStr">
@@ -12998,7 +12998,7 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H349" t="inlineStr">
@@ -13070,7 +13070,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -13142,7 +13142,7 @@
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H353" t="inlineStr">
@@ -13214,7 +13214,7 @@
       </c>
       <c r="G355" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H355" t="inlineStr">
@@ -13250,7 +13250,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -13358,7 +13358,7 @@
       </c>
       <c r="G359" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H359" t="inlineStr">
@@ -13394,7 +13394,7 @@
       </c>
       <c r="G360" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H360" t="inlineStr">
@@ -13574,7 +13574,7 @@
       </c>
       <c r="G365" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H365" t="inlineStr">
@@ -13646,7 +13646,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H367" t="inlineStr">
@@ -13754,7 +13754,7 @@
       </c>
       <c r="G370" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H370" t="inlineStr">
@@ -13826,7 +13826,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H372" t="inlineStr">
@@ -14222,7 +14222,7 @@
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H383" t="inlineStr">
@@ -14258,7 +14258,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -14294,7 +14294,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H385" t="inlineStr">
@@ -14438,7 +14438,7 @@
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H389" t="inlineStr">
@@ -14474,7 +14474,7 @@
       </c>
       <c r="G390" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H390" t="inlineStr">
@@ -14546,7 +14546,7 @@
       </c>
       <c r="G392" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H392" t="inlineStr">
@@ -14726,7 +14726,7 @@
       </c>
       <c r="G397" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H397" t="inlineStr">
@@ -14798,7 +14798,7 @@
       </c>
       <c r="G399" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H399" t="inlineStr">
@@ -14834,7 +14834,7 @@
       </c>
       <c r="G400" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H400" t="inlineStr">
@@ -15122,7 +15122,7 @@
       </c>
       <c r="G408" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H408" t="inlineStr">
@@ -15158,7 +15158,7 @@
       </c>
       <c r="G409" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H409" t="inlineStr">
@@ -15194,7 +15194,7 @@
       </c>
       <c r="G410" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H410" t="inlineStr">
@@ -15302,7 +15302,7 @@
       </c>
       <c r="G413" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H413" t="inlineStr">
@@ -15554,7 +15554,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H420" t="inlineStr">
@@ -15590,7 +15590,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H421" t="inlineStr">
@@ -15626,7 +15626,7 @@
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H422" t="inlineStr">
@@ -15662,7 +15662,7 @@
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H423" t="inlineStr">
@@ -15806,7 +15806,7 @@
       </c>
       <c r="G427" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H427" t="inlineStr">
@@ -15950,7 +15950,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H431" t="inlineStr">
@@ -16058,7 +16058,7 @@
       </c>
       <c r="G434" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H434" t="inlineStr">
@@ -16166,7 +16166,7 @@
       </c>
       <c r="G437" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H437" t="inlineStr">
@@ -16310,7 +16310,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H441" t="inlineStr">
@@ -16346,7 +16346,7 @@
       </c>
       <c r="G442" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H442" t="inlineStr">
@@ -16382,7 +16382,7 @@
       </c>
       <c r="G443" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H443" t="inlineStr">
@@ -16634,7 +16634,7 @@
       </c>
       <c r="G450" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H450" t="inlineStr">
@@ -17066,7 +17066,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H462" t="inlineStr">
@@ -17246,7 +17246,7 @@
       </c>
       <c r="G467" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H467" t="inlineStr">
@@ -17282,7 +17282,7 @@
       </c>
       <c r="G468" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H468" t="inlineStr">
@@ -17318,7 +17318,7 @@
       </c>
       <c r="G469" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H469" t="inlineStr">
@@ -17354,7 +17354,7 @@
       </c>
       <c r="G470" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H470" t="inlineStr">
@@ -17426,7 +17426,7 @@
       </c>
       <c r="G472" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H472" t="inlineStr">
@@ -17498,7 +17498,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Investing Activities (Rule)</t>
         </is>
       </c>
       <c r="H474" t="inlineStr">
@@ -17534,7 +17534,7 @@
       </c>
       <c r="G475" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H475" t="inlineStr">
@@ -17570,7 +17570,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H476" t="inlineStr">
@@ -17606,7 +17606,7 @@
       </c>
       <c r="G477" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H477" t="inlineStr">
@@ -17642,7 +17642,7 @@
       </c>
       <c r="G478" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H478" t="inlineStr">
@@ -17678,7 +17678,7 @@
       </c>
       <c r="G479" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H479" t="inlineStr">
@@ -17786,7 +17786,7 @@
       </c>
       <c r="G482" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H482" t="inlineStr">
@@ -17822,7 +17822,7 @@
       </c>
       <c r="G483" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule)</t>
         </is>
       </c>
       <c r="H483" t="inlineStr">
@@ -18002,7 +18002,7 @@
       </c>
       <c r="G488" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H488" t="inlineStr">
@@ -18074,7 +18074,7 @@
       </c>
       <c r="G490" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule)</t>
         </is>
       </c>
       <c r="H490" t="inlineStr">

</xml_diff>

<commit_message>
Vendor wise breakdown..download button not working in this
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -578,7 +578,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -722,7 +722,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -758,7 +758,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -830,7 +830,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1802,7 +1802,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2054,7 +2054,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2162,7 +2162,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -2666,7 +2666,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -2774,7 +2774,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -3278,7 +3278,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -3314,7 +3314,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -3422,7 +3422,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -3602,7 +3602,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -3782,7 +3782,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -3854,7 +3854,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -3962,7 +3962,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -4142,7 +4142,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -4214,7 +4214,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -4322,7 +4322,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -4430,7 +4430,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -4502,7 +4502,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -4538,7 +4538,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -4682,7 +4682,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
@@ -4754,7 +4754,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -4790,7 +4790,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -4826,7 +4826,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
@@ -4862,7 +4862,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -4934,7 +4934,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -4970,7 +4970,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -5006,7 +5006,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
@@ -5078,7 +5078,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
@@ -5114,7 +5114,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
@@ -5186,7 +5186,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -5258,7 +5258,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
@@ -5330,7 +5330,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -5366,7 +5366,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -5402,7 +5402,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -5474,7 +5474,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
@@ -5510,7 +5510,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -5582,7 +5582,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
@@ -5654,7 +5654,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
@@ -5690,7 +5690,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -5762,7 +5762,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -5798,7 +5798,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
@@ -5834,7 +5834,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -5870,7 +5870,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
@@ -5942,7 +5942,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
@@ -5978,7 +5978,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
@@ -6014,7 +6014,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -6086,7 +6086,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
@@ -6122,7 +6122,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
@@ -6158,7 +6158,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -6194,7 +6194,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
@@ -6410,7 +6410,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -6518,7 +6518,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
@@ -6554,7 +6554,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
@@ -6590,7 +6590,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -6626,7 +6626,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
@@ -6662,7 +6662,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H174" t="inlineStr">
@@ -6734,7 +6734,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -6770,7 +6770,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -6842,7 +6842,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
@@ -6878,7 +6878,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
@@ -6914,7 +6914,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
@@ -6950,7 +6950,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -6986,7 +6986,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
@@ -7022,7 +7022,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
@@ -7130,7 +7130,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
@@ -7202,7 +7202,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
@@ -7274,7 +7274,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
@@ -7310,7 +7310,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -7346,7 +7346,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
@@ -7382,7 +7382,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -7418,7 +7418,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -7490,7 +7490,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -7526,7 +7526,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -7562,7 +7562,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
@@ -7598,7 +7598,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -7634,7 +7634,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
@@ -7670,7 +7670,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -7706,7 +7706,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
@@ -7742,7 +7742,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
@@ -7778,7 +7778,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -7814,7 +7814,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
@@ -7850,7 +7850,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -7922,7 +7922,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
@@ -7958,7 +7958,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -7994,7 +7994,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -8030,7 +8030,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -8066,7 +8066,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
@@ -8102,7 +8102,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -8138,7 +8138,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
@@ -8174,7 +8174,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
@@ -8210,7 +8210,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
@@ -8246,7 +8246,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -8282,7 +8282,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
@@ -8318,7 +8318,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
@@ -8354,7 +8354,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
@@ -8390,7 +8390,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -8426,7 +8426,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -8462,7 +8462,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -8498,7 +8498,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
@@ -8534,7 +8534,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -8570,7 +8570,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -8606,7 +8606,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
@@ -8642,7 +8642,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
@@ -8678,7 +8678,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
@@ -8714,7 +8714,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
@@ -8750,7 +8750,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -8786,7 +8786,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
@@ -8822,7 +8822,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -8858,7 +8858,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -8894,7 +8894,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
@@ -8930,7 +8930,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -8966,7 +8966,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
@@ -9002,7 +9002,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
@@ -9038,7 +9038,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
@@ -9074,7 +9074,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -9110,7 +9110,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -9146,7 +9146,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
@@ -9182,7 +9182,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
@@ -9218,7 +9218,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
@@ -9254,7 +9254,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
@@ -9290,7 +9290,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -9326,7 +9326,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
@@ -9362,7 +9362,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
@@ -9398,7 +9398,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -9434,7 +9434,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
@@ -9470,7 +9470,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -9506,7 +9506,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
@@ -9542,7 +9542,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
@@ -9578,7 +9578,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
@@ -9614,7 +9614,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
@@ -9650,7 +9650,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -9686,7 +9686,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
@@ -9722,7 +9722,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
@@ -9758,7 +9758,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
@@ -9794,7 +9794,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
@@ -9830,7 +9830,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
@@ -9866,7 +9866,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
@@ -9902,7 +9902,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
@@ -9938,7 +9938,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H264" t="inlineStr">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H265" t="inlineStr">
@@ -10010,7 +10010,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -10046,7 +10046,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
@@ -10082,7 +10082,7 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H268" t="inlineStr">
@@ -10118,7 +10118,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H269" t="inlineStr">
@@ -10154,7 +10154,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H270" t="inlineStr">
@@ -10190,7 +10190,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -10226,7 +10226,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H272" t="inlineStr">
@@ -10262,7 +10262,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H273" t="inlineStr">
@@ -10298,7 +10298,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
@@ -10334,7 +10334,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H275" t="inlineStr">
@@ -10370,7 +10370,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -10406,7 +10406,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H277" t="inlineStr">
@@ -10442,7 +10442,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H278" t="inlineStr">
@@ -10478,7 +10478,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H279" t="inlineStr">
@@ -10514,7 +10514,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
@@ -10550,7 +10550,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -10586,7 +10586,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H282" t="inlineStr">
@@ -10658,7 +10658,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H284" t="inlineStr">
@@ -10694,7 +10694,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -10730,7 +10730,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
@@ -10766,7 +10766,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H287" t="inlineStr">
@@ -10802,7 +10802,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H288" t="inlineStr">
@@ -10838,7 +10838,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H289" t="inlineStr">
@@ -10874,7 +10874,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
@@ -10910,7 +10910,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -10946,7 +10946,7 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H292" t="inlineStr">
@@ -10982,7 +10982,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
@@ -11018,7 +11018,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
@@ -11054,7 +11054,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
@@ -11090,7 +11090,7 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H296" t="inlineStr">
@@ -11126,7 +11126,7 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H297" t="inlineStr">
@@ -11162,7 +11162,7 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H298" t="inlineStr">
@@ -11198,7 +11198,7 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H299" t="inlineStr">
@@ -11234,7 +11234,7 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H300" t="inlineStr">
@@ -11306,7 +11306,7 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H302" t="inlineStr">
@@ -11342,7 +11342,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -11378,7 +11378,7 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H304" t="inlineStr">
@@ -11414,7 +11414,7 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H305" t="inlineStr">
@@ -11450,7 +11450,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -11486,7 +11486,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
@@ -11522,7 +11522,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H308" t="inlineStr">
@@ -11558,7 +11558,7 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H309" t="inlineStr">
@@ -11594,7 +11594,7 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H310" t="inlineStr">
@@ -11630,7 +11630,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
@@ -11666,7 +11666,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H312" t="inlineStr">
@@ -11702,7 +11702,7 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H313" t="inlineStr">
@@ -11738,7 +11738,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H314" t="inlineStr">
@@ -11774,7 +11774,7 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H315" t="inlineStr">
@@ -11810,7 +11810,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -11846,7 +11846,7 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H317" t="inlineStr">
@@ -11882,7 +11882,7 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H318" t="inlineStr">
@@ -11918,7 +11918,7 @@
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H319" t="inlineStr">
@@ -11954,7 +11954,7 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H320" t="inlineStr">
@@ -11990,7 +11990,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -12026,7 +12026,7 @@
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H322" t="inlineStr">
@@ -12062,7 +12062,7 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H323" t="inlineStr">
@@ -12098,7 +12098,7 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H324" t="inlineStr">
@@ -12134,7 +12134,7 @@
       </c>
       <c r="G325" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H325" t="inlineStr">
@@ -12170,7 +12170,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -12242,7 +12242,7 @@
       </c>
       <c r="G328" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H328" t="inlineStr">
@@ -12278,7 +12278,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H329" t="inlineStr">
@@ -12314,7 +12314,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H330" t="inlineStr">
@@ -12350,7 +12350,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H331" t="inlineStr">
@@ -12386,7 +12386,7 @@
       </c>
       <c r="G332" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H332" t="inlineStr">
@@ -12422,7 +12422,7 @@
       </c>
       <c r="G333" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H333" t="inlineStr">
@@ -12458,7 +12458,7 @@
       </c>
       <c r="G334" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H334" t="inlineStr">
@@ -12494,7 +12494,7 @@
       </c>
       <c r="G335" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H335" t="inlineStr">
@@ -12530,7 +12530,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H336" t="inlineStr">
@@ -12566,7 +12566,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H337" t="inlineStr">
@@ -12602,7 +12602,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H338" t="inlineStr">
@@ -12638,7 +12638,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H339" t="inlineStr">
@@ -12674,7 +12674,7 @@
       </c>
       <c r="G340" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H340" t="inlineStr">
@@ -12710,7 +12710,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H341" t="inlineStr">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="G342" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H342" t="inlineStr">
@@ -12782,7 +12782,7 @@
       </c>
       <c r="G343" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H343" t="inlineStr">
@@ -12818,7 +12818,7 @@
       </c>
       <c r="G344" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H344" t="inlineStr">
@@ -12854,7 +12854,7 @@
       </c>
       <c r="G345" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H345" t="inlineStr">
@@ -12890,7 +12890,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H346" t="inlineStr">
@@ -12926,7 +12926,7 @@
       </c>
       <c r="G347" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H347" t="inlineStr">
@@ -12962,7 +12962,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -12998,7 +12998,7 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H349" t="inlineStr">
@@ -13070,7 +13070,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -13106,7 +13106,7 @@
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H352" t="inlineStr">
@@ -13178,7 +13178,7 @@
       </c>
       <c r="G354" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H354" t="inlineStr">
@@ -13214,7 +13214,7 @@
       </c>
       <c r="G355" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H355" t="inlineStr">
@@ -13250,7 +13250,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -13286,7 +13286,7 @@
       </c>
       <c r="G357" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H357" t="inlineStr">
@@ -13322,7 +13322,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H358" t="inlineStr">
@@ -13358,7 +13358,7 @@
       </c>
       <c r="G359" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H359" t="inlineStr">
@@ -13394,7 +13394,7 @@
       </c>
       <c r="G360" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H360" t="inlineStr">
@@ -13430,7 +13430,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H361" t="inlineStr">
@@ -13466,7 +13466,7 @@
       </c>
       <c r="G362" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H362" t="inlineStr">
@@ -13502,7 +13502,7 @@
       </c>
       <c r="G363" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H363" t="inlineStr">
@@ -13538,7 +13538,7 @@
       </c>
       <c r="G364" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H364" t="inlineStr">
@@ -13574,7 +13574,7 @@
       </c>
       <c r="G365" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H365" t="inlineStr">
@@ -13610,7 +13610,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -13646,7 +13646,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H367" t="inlineStr">
@@ -13682,7 +13682,7 @@
       </c>
       <c r="G368" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H368" t="inlineStr">
@@ -13718,7 +13718,7 @@
       </c>
       <c r="G369" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H369" t="inlineStr">
@@ -13754,7 +13754,7 @@
       </c>
       <c r="G370" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H370" t="inlineStr">
@@ -13790,7 +13790,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H371" t="inlineStr">
@@ -13826,7 +13826,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H372" t="inlineStr">
@@ -13862,7 +13862,7 @@
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H373" t="inlineStr">
@@ -13898,7 +13898,7 @@
       </c>
       <c r="G374" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H374" t="inlineStr">
@@ -13934,7 +13934,7 @@
       </c>
       <c r="G375" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H375" t="inlineStr">
@@ -13970,7 +13970,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H376" t="inlineStr">
@@ -14006,7 +14006,7 @@
       </c>
       <c r="G377" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H377" t="inlineStr">
@@ -14042,7 +14042,7 @@
       </c>
       <c r="G378" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H378" t="inlineStr">
@@ -14078,7 +14078,7 @@
       </c>
       <c r="G379" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H379" t="inlineStr">
@@ -14114,7 +14114,7 @@
       </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H380" t="inlineStr">
@@ -14150,7 +14150,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -14186,7 +14186,7 @@
       </c>
       <c r="G382" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H382" t="inlineStr">
@@ -14222,7 +14222,7 @@
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H383" t="inlineStr">
@@ -14258,7 +14258,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -14294,7 +14294,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H385" t="inlineStr">
@@ -14330,7 +14330,7 @@
       </c>
       <c r="G386" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H386" t="inlineStr">
@@ -14366,7 +14366,7 @@
       </c>
       <c r="G387" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H387" t="inlineStr">
@@ -14402,7 +14402,7 @@
       </c>
       <c r="G388" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H388" t="inlineStr">
@@ -14438,7 +14438,7 @@
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H389" t="inlineStr">
@@ -14474,7 +14474,7 @@
       </c>
       <c r="G390" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H390" t="inlineStr">
@@ -14510,7 +14510,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H391" t="inlineStr">
@@ -14546,7 +14546,7 @@
       </c>
       <c r="G392" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H392" t="inlineStr">
@@ -14582,7 +14582,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -14618,7 +14618,7 @@
       </c>
       <c r="G394" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H394" t="inlineStr">
@@ -14654,7 +14654,7 @@
       </c>
       <c r="G395" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H395" t="inlineStr">
@@ -14690,7 +14690,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H396" t="inlineStr">
@@ -14726,7 +14726,7 @@
       </c>
       <c r="G397" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H397" t="inlineStr">
@@ -14762,7 +14762,7 @@
       </c>
       <c r="G398" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H398" t="inlineStr">
@@ -14834,7 +14834,7 @@
       </c>
       <c r="G400" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H400" t="inlineStr">
@@ -14870,7 +14870,7 @@
       </c>
       <c r="G401" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H401" t="inlineStr">
@@ -14906,7 +14906,7 @@
       </c>
       <c r="G402" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H402" t="inlineStr">
@@ -14942,7 +14942,7 @@
       </c>
       <c r="G403" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H403" t="inlineStr">
@@ -14978,7 +14978,7 @@
       </c>
       <c r="G404" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H404" t="inlineStr">
@@ -15014,7 +15014,7 @@
       </c>
       <c r="G405" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H405" t="inlineStr">
@@ -15050,7 +15050,7 @@
       </c>
       <c r="G406" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H406" t="inlineStr">
@@ -15086,7 +15086,7 @@
       </c>
       <c r="G407" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H407" t="inlineStr">
@@ -15122,7 +15122,7 @@
       </c>
       <c r="G408" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H408" t="inlineStr">
@@ -15158,7 +15158,7 @@
       </c>
       <c r="G409" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H409" t="inlineStr">
@@ -15194,7 +15194,7 @@
       </c>
       <c r="G410" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H410" t="inlineStr">
@@ -15230,7 +15230,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -15266,7 +15266,7 @@
       </c>
       <c r="G412" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H412" t="inlineStr">
@@ -15302,7 +15302,7 @@
       </c>
       <c r="G413" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H413" t="inlineStr">
@@ -15338,7 +15338,7 @@
       </c>
       <c r="G414" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H414" t="inlineStr">
@@ -15374,7 +15374,7 @@
       </c>
       <c r="G415" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H415" t="inlineStr">
@@ -15410,7 +15410,7 @@
       </c>
       <c r="G416" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H416" t="inlineStr">
@@ -15446,7 +15446,7 @@
       </c>
       <c r="G417" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H417" t="inlineStr">
@@ -15482,7 +15482,7 @@
       </c>
       <c r="G418" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H418" t="inlineStr">
@@ -15518,7 +15518,7 @@
       </c>
       <c r="G419" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H419" t="inlineStr">
@@ -15554,7 +15554,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H420" t="inlineStr">
@@ -15590,7 +15590,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H421" t="inlineStr">
@@ -15626,7 +15626,7 @@
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H422" t="inlineStr">
@@ -15662,7 +15662,7 @@
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H423" t="inlineStr">
@@ -15698,7 +15698,7 @@
       </c>
       <c r="G424" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H424" t="inlineStr">
@@ -15770,7 +15770,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H426" t="inlineStr">
@@ -15842,7 +15842,7 @@
       </c>
       <c r="G428" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H428" t="inlineStr">
@@ -15878,7 +15878,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H429" t="inlineStr">
@@ -15914,7 +15914,7 @@
       </c>
       <c r="G430" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H430" t="inlineStr">
@@ -15986,7 +15986,7 @@
       </c>
       <c r="G432" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H432" t="inlineStr">
@@ -16022,7 +16022,7 @@
       </c>
       <c r="G433" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H433" t="inlineStr">
@@ -16058,7 +16058,7 @@
       </c>
       <c r="G434" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H434" t="inlineStr">
@@ -16094,7 +16094,7 @@
       </c>
       <c r="G435" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H435" t="inlineStr">
@@ -16166,7 +16166,7 @@
       </c>
       <c r="G437" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H437" t="inlineStr">
@@ -16202,7 +16202,7 @@
       </c>
       <c r="G438" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H438" t="inlineStr">
@@ -16238,7 +16238,7 @@
       </c>
       <c r="G439" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H439" t="inlineStr">
@@ -16274,7 +16274,7 @@
       </c>
       <c r="G440" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H440" t="inlineStr">
@@ -16310,7 +16310,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H441" t="inlineStr">
@@ -16346,7 +16346,7 @@
       </c>
       <c r="G442" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H442" t="inlineStr">
@@ -16382,7 +16382,7 @@
       </c>
       <c r="G443" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H443" t="inlineStr">
@@ -16418,7 +16418,7 @@
       </c>
       <c r="G444" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H444" t="inlineStr">
@@ -16454,7 +16454,7 @@
       </c>
       <c r="G445" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H445" t="inlineStr">
@@ -16490,7 +16490,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H446" t="inlineStr">
@@ -16526,7 +16526,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H447" t="inlineStr">
@@ -16562,7 +16562,7 @@
       </c>
       <c r="G448" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H448" t="inlineStr">
@@ -16598,7 +16598,7 @@
       </c>
       <c r="G449" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H449" t="inlineStr">
@@ -16634,7 +16634,7 @@
       </c>
       <c r="G450" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H450" t="inlineStr">
@@ -16670,7 +16670,7 @@
       </c>
       <c r="G451" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H451" t="inlineStr">
@@ -16706,7 +16706,7 @@
       </c>
       <c r="G452" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H452" t="inlineStr">
@@ -16742,7 +16742,7 @@
       </c>
       <c r="G453" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H453" t="inlineStr">
@@ -16778,7 +16778,7 @@
       </c>
       <c r="G454" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H454" t="inlineStr">
@@ -16814,7 +16814,7 @@
       </c>
       <c r="G455" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H455" t="inlineStr">
@@ -16850,7 +16850,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H456" t="inlineStr">
@@ -16886,7 +16886,7 @@
       </c>
       <c r="G457" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H457" t="inlineStr">
@@ -16922,7 +16922,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H458" t="inlineStr">
@@ -16958,7 +16958,7 @@
       </c>
       <c r="G459" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H459" t="inlineStr">
@@ -16994,7 +16994,7 @@
       </c>
       <c r="G460" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H460" t="inlineStr">
@@ -17030,7 +17030,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H461" t="inlineStr">
@@ -17066,7 +17066,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H462" t="inlineStr">
@@ -17102,7 +17102,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H463" t="inlineStr">
@@ -17138,7 +17138,7 @@
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H464" t="inlineStr">
@@ -17174,7 +17174,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H465" t="inlineStr">
@@ -17210,7 +17210,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H466" t="inlineStr">
@@ -17246,7 +17246,7 @@
       </c>
       <c r="G467" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H467" t="inlineStr">
@@ -17282,7 +17282,7 @@
       </c>
       <c r="G468" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H468" t="inlineStr">
@@ -17318,7 +17318,7 @@
       </c>
       <c r="G469" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H469" t="inlineStr">
@@ -17354,7 +17354,7 @@
       </c>
       <c r="G470" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H470" t="inlineStr">
@@ -17390,7 +17390,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H471" t="inlineStr">
@@ -17426,7 +17426,7 @@
       </c>
       <c r="G472" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H472" t="inlineStr">
@@ -17462,7 +17462,7 @@
       </c>
       <c r="G473" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H473" t="inlineStr">
@@ -17498,7 +17498,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H474" t="inlineStr">
@@ -17534,7 +17534,7 @@
       </c>
       <c r="G475" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H475" t="inlineStr">
@@ -17570,7 +17570,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H476" t="inlineStr">
@@ -17606,7 +17606,7 @@
       </c>
       <c r="G477" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H477" t="inlineStr">
@@ -17678,7 +17678,7 @@
       </c>
       <c r="G479" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H479" t="inlineStr">
@@ -17714,7 +17714,7 @@
       </c>
       <c r="G480" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (AI)</t>
         </is>
       </c>
       <c r="H480" t="inlineStr">
@@ -17750,7 +17750,7 @@
       </c>
       <c r="G481" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H481" t="inlineStr">
@@ -17822,7 +17822,7 @@
       </c>
       <c r="G483" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H483" t="inlineStr">
@@ -17858,7 +17858,7 @@
       </c>
       <c r="G484" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H484" t="inlineStr">
@@ -17894,7 +17894,7 @@
       </c>
       <c r="G485" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H485" t="inlineStr">
@@ -17930,7 +17930,7 @@
       </c>
       <c r="G486" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H486" t="inlineStr">
@@ -17966,7 +17966,7 @@
       </c>
       <c r="G487" t="inlineStr">
         <is>
-          <t>Investing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H487" t="inlineStr">
@@ -18002,7 +18002,7 @@
       </c>
       <c r="G488" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H488" t="inlineStr">
@@ -18038,7 +18038,7 @@
       </c>
       <c r="G489" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H489" t="inlineStr">
@@ -18074,7 +18074,7 @@
       </c>
       <c r="G490" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H490" t="inlineStr">
@@ -18110,7 +18110,7 @@
       </c>
       <c r="G491" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Financing Activities (AI)</t>
         </is>
       </c>
       <c r="H491" t="inlineStr">
@@ -18146,7 +18146,7 @@
       </c>
       <c r="G492" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H492" t="inlineStr">
@@ -18182,7 +18182,7 @@
       </c>
       <c r="G493" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H493" t="inlineStr">
@@ -18216,7 +18216,7 @@
       <c r="F494" t="inlineStr"/>
       <c r="G494" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H494" t="inlineStr">

</xml_diff>

<commit_message>
cashflow and vendor analysis - changes made as there is a difference,vendor analysis button not working
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -830,7 +830,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -4682,7 +4682,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
@@ -4862,7 +4862,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -4898,7 +4898,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -5258,7 +5258,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -5510,7 +5510,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -5762,7 +5762,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -5870,7 +5870,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -6266,7 +6266,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -6482,7 +6482,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -6518,7 +6518,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
@@ -7022,7 +7022,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
@@ -7094,7 +7094,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -7382,7 +7382,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -7670,7 +7670,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -7742,7 +7742,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
@@ -7778,7 +7778,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -7850,7 +7850,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -7886,7 +7886,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
@@ -7958,7 +7958,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -8102,7 +8102,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -8354,7 +8354,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
@@ -8570,7 +8570,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -8606,7 +8606,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
@@ -8750,7 +8750,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -8822,7 +8822,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -8858,7 +8858,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -9434,7 +9434,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
@@ -10046,7 +10046,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
@@ -10118,7 +10118,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H269" t="inlineStr">
@@ -10226,7 +10226,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H272" t="inlineStr">
@@ -10298,7 +10298,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
@@ -10334,7 +10334,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H275" t="inlineStr">
@@ -10478,7 +10478,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H279" t="inlineStr">
@@ -10514,7 +10514,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
@@ -10622,7 +10622,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H283" t="inlineStr">
@@ -10874,7 +10874,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
@@ -10910,7 +10910,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -11054,7 +11054,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
@@ -11270,7 +11270,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -11414,7 +11414,7 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H305" t="inlineStr">
@@ -11702,7 +11702,7 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H313" t="inlineStr">
@@ -11738,7 +11738,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H314" t="inlineStr">
@@ -11882,7 +11882,7 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H318" t="inlineStr">
@@ -12206,7 +12206,7 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H327" t="inlineStr">
@@ -12386,7 +12386,7 @@
       </c>
       <c r="G332" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Payroll)</t>
         </is>
       </c>
       <c r="H332" t="inlineStr">
@@ -12458,7 +12458,7 @@
       </c>
       <c r="G334" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H334" t="inlineStr">
@@ -12602,7 +12602,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H338" t="inlineStr">
@@ -12674,7 +12674,7 @@
       </c>
       <c r="G340" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H340" t="inlineStr">
@@ -12962,7 +12962,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -13034,7 +13034,7 @@
       </c>
       <c r="G350" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H350" t="inlineStr">
@@ -13142,7 +13142,7 @@
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H353" t="inlineStr">
@@ -13322,7 +13322,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H358" t="inlineStr">
@@ -13430,7 +13430,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H361" t="inlineStr">
@@ -13862,7 +13862,7 @@
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H373" t="inlineStr">
@@ -14006,7 +14006,7 @@
       </c>
       <c r="G377" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H377" t="inlineStr">
@@ -14078,7 +14078,7 @@
       </c>
       <c r="G379" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H379" t="inlineStr">
@@ -14222,7 +14222,7 @@
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H383" t="inlineStr">
@@ -14294,7 +14294,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H385" t="inlineStr">
@@ -14582,7 +14582,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -14798,7 +14798,7 @@
       </c>
       <c r="G399" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H399" t="inlineStr">
@@ -15014,7 +15014,7 @@
       </c>
       <c r="G405" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H405" t="inlineStr">
@@ -15698,7 +15698,7 @@
       </c>
       <c r="G424" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H424" t="inlineStr">
@@ -15734,7 +15734,7 @@
       </c>
       <c r="G425" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H425" t="inlineStr">
@@ -15806,7 +15806,7 @@
       </c>
       <c r="G427" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Vendor)</t>
         </is>
       </c>
       <c r="H427" t="inlineStr">
@@ -15950,7 +15950,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Financing Activities (Rule-Finance)</t>
         </is>
       </c>
       <c r="H431" t="inlineStr">
@@ -16130,7 +16130,7 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H436" t="inlineStr">
@@ -16238,7 +16238,7 @@
       </c>
       <c r="G439" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H439" t="inlineStr">
@@ -16382,7 +16382,7 @@
       </c>
       <c r="G443" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H443" t="inlineStr">
@@ -16490,7 +16490,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H446" t="inlineStr">
@@ -16670,7 +16670,7 @@
       </c>
       <c r="G451" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H451" t="inlineStr">
@@ -16886,7 +16886,7 @@
       </c>
       <c r="G457" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H457" t="inlineStr">
@@ -17102,7 +17102,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H463" t="inlineStr">
@@ -17534,7 +17534,7 @@
       </c>
       <c r="G475" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H475" t="inlineStr">
@@ -17642,7 +17642,7 @@
       </c>
       <c r="G478" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H478" t="inlineStr">
@@ -17714,7 +17714,7 @@
       </c>
       <c r="G480" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H480" t="inlineStr">
@@ -17786,7 +17786,7 @@
       </c>
       <c r="G482" t="inlineStr">
         <is>
-          <t>Operating Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H482" t="inlineStr">
@@ -17858,7 +17858,7 @@
       </c>
       <c r="G484" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Operating Activities (Rule-Utility)</t>
         </is>
       </c>
       <c r="H484" t="inlineStr">
@@ -18110,7 +18110,7 @@
       </c>
       <c r="G491" t="inlineStr">
         <is>
-          <t>Financing Activities (AI)</t>
+          <t>Operating Activities (Rule-Default)</t>
         </is>
       </c>
       <c r="H491" t="inlineStr">

</xml_diff>

<commit_message>
UI Changes and Open ai api prompt changes
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -578,7 +578,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -722,7 +722,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -758,7 +758,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -830,7 +830,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Payroll)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1802,7 +1802,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2054,7 +2054,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2162,7 +2162,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Payroll)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Operating Activities (AI-Detailed)</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -2666,7 +2666,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -2774,7 +2774,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -3278,7 +3278,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -3422,7 +3422,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -3602,7 +3602,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -3962,7 +3962,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -4214,7 +4214,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
@@ -4754,7 +4754,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -4790,7 +4790,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -4862,7 +4862,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -4970,7 +4970,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -5006,7 +5006,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -5150,7 +5150,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
@@ -5330,7 +5330,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -5366,7 +5366,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -5438,7 +5438,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -5474,7 +5474,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
@@ -5510,7 +5510,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -5582,7 +5582,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -5762,7 +5762,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
@@ -6014,7 +6014,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -6122,7 +6122,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
@@ -6158,7 +6158,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -6194,7 +6194,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
@@ -6410,7 +6410,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -6590,7 +6590,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -6662,7 +6662,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
@@ -6734,7 +6734,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -6770,7 +6770,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -6842,7 +6842,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
@@ -6986,7 +6986,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
@@ -7022,7 +7022,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
@@ -7094,7 +7094,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
@@ -7130,7 +7130,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -7202,7 +7202,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
@@ -7238,7 +7238,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
@@ -7274,7 +7274,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
@@ -7382,7 +7382,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -7418,7 +7418,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -7490,7 +7490,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -7526,7 +7526,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -7598,7 +7598,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -7670,7 +7670,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -7706,7 +7706,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
@@ -7742,7 +7742,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
@@ -7778,7 +7778,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -7814,7 +7814,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
@@ -7886,7 +7886,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
@@ -7994,7 +7994,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -8066,7 +8066,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
@@ -8102,7 +8102,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -8138,7 +8138,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
@@ -8246,7 +8246,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -8282,7 +8282,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
@@ -8318,7 +8318,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
@@ -8354,7 +8354,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
@@ -8462,7 +8462,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -8498,7 +8498,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
@@ -8570,7 +8570,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -8642,7 +8642,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
@@ -8678,7 +8678,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
@@ -8786,7 +8786,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
@@ -8822,7 +8822,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -8858,7 +8858,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -8966,7 +8966,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
@@ -9002,7 +9002,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
@@ -9038,7 +9038,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
@@ -9110,7 +9110,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -9182,7 +9182,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
@@ -9218,7 +9218,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
@@ -9254,7 +9254,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
@@ -9290,7 +9290,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -9362,7 +9362,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
@@ -9398,7 +9398,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -9470,7 +9470,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -9506,7 +9506,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
@@ -9614,7 +9614,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
@@ -9686,7 +9686,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
@@ -9722,7 +9722,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
@@ -9794,7 +9794,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
@@ -9830,7 +9830,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
@@ -9938,7 +9938,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H264" t="inlineStr">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H265" t="inlineStr">
@@ -10154,7 +10154,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H270" t="inlineStr">
@@ -10226,7 +10226,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H272" t="inlineStr">
@@ -10334,7 +10334,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H275" t="inlineStr">
@@ -10370,7 +10370,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -10406,7 +10406,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H277" t="inlineStr">
@@ -10442,7 +10442,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H278" t="inlineStr">
@@ -10478,7 +10478,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H279" t="inlineStr">
@@ -10514,7 +10514,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
@@ -10586,7 +10586,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H282" t="inlineStr">
@@ -10622,7 +10622,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H283" t="inlineStr">
@@ -10658,7 +10658,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H284" t="inlineStr">
@@ -10766,7 +10766,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H287" t="inlineStr">
@@ -10802,7 +10802,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H288" t="inlineStr">
@@ -10838,7 +10838,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H289" t="inlineStr">
@@ -10874,7 +10874,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
@@ -10910,7 +10910,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -10982,7 +10982,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
@@ -11018,7 +11018,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
@@ -11054,7 +11054,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
@@ -11198,7 +11198,7 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H299" t="inlineStr">
@@ -11270,7 +11270,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -11306,7 +11306,7 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H302" t="inlineStr">
@@ -11342,7 +11342,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -11450,7 +11450,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -11486,7 +11486,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
@@ -11522,7 +11522,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H308" t="inlineStr">
@@ -11558,7 +11558,7 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H309" t="inlineStr">
@@ -11630,7 +11630,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
@@ -11738,7 +11738,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H314" t="inlineStr">
@@ -11810,7 +11810,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -11846,7 +11846,7 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H317" t="inlineStr">
@@ -11882,7 +11882,7 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H318" t="inlineStr">
@@ -11954,7 +11954,7 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H320" t="inlineStr">
@@ -12062,7 +12062,7 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H323" t="inlineStr">
@@ -12134,7 +12134,7 @@
       </c>
       <c r="G325" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H325" t="inlineStr">
@@ -12170,7 +12170,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -12206,7 +12206,7 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H327" t="inlineStr">
@@ -12242,7 +12242,7 @@
       </c>
       <c r="G328" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H328" t="inlineStr">
@@ -12278,7 +12278,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H329" t="inlineStr">
@@ -12350,7 +12350,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H331" t="inlineStr">
@@ -12422,7 +12422,7 @@
       </c>
       <c r="G333" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H333" t="inlineStr">
@@ -12458,7 +12458,7 @@
       </c>
       <c r="G334" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H334" t="inlineStr">
@@ -12494,7 +12494,7 @@
       </c>
       <c r="G335" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H335" t="inlineStr">
@@ -12530,7 +12530,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H336" t="inlineStr">
@@ -12602,7 +12602,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H338" t="inlineStr">
@@ -12674,7 +12674,7 @@
       </c>
       <c r="G340" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H340" t="inlineStr">
@@ -12710,7 +12710,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H341" t="inlineStr">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="G342" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H342" t="inlineStr">
@@ -12818,7 +12818,7 @@
       </c>
       <c r="G344" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H344" t="inlineStr">
@@ -12854,7 +12854,7 @@
       </c>
       <c r="G345" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H345" t="inlineStr">
@@ -12926,7 +12926,7 @@
       </c>
       <c r="G347" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H347" t="inlineStr">
@@ -12962,7 +12962,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -12998,7 +12998,7 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H349" t="inlineStr">
@@ -13034,7 +13034,7 @@
       </c>
       <c r="G350" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H350" t="inlineStr">
@@ -13070,7 +13070,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -13106,7 +13106,7 @@
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H352" t="inlineStr">
@@ -13286,7 +13286,7 @@
       </c>
       <c r="G357" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H357" t="inlineStr">
@@ -13322,7 +13322,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H358" t="inlineStr">
@@ -13394,7 +13394,7 @@
       </c>
       <c r="G360" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H360" t="inlineStr">
@@ -13430,7 +13430,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H361" t="inlineStr">
@@ -13466,7 +13466,7 @@
       </c>
       <c r="G362" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H362" t="inlineStr">
@@ -13502,7 +13502,7 @@
       </c>
       <c r="G363" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H363" t="inlineStr">
@@ -13538,7 +13538,7 @@
       </c>
       <c r="G364" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H364" t="inlineStr">
@@ -13574,7 +13574,7 @@
       </c>
       <c r="G365" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H365" t="inlineStr">
@@ -13610,7 +13610,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -13646,7 +13646,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H367" t="inlineStr">
@@ -13682,7 +13682,7 @@
       </c>
       <c r="G368" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H368" t="inlineStr">
@@ -13754,7 +13754,7 @@
       </c>
       <c r="G370" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H370" t="inlineStr">
@@ -13790,7 +13790,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H371" t="inlineStr">
@@ -13934,7 +13934,7 @@
       </c>
       <c r="G375" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H375" t="inlineStr">
@@ -13970,7 +13970,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H376" t="inlineStr">
@@ -14114,7 +14114,7 @@
       </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H380" t="inlineStr">
@@ -14150,7 +14150,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -14258,7 +14258,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -14294,7 +14294,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H385" t="inlineStr">
@@ -14402,7 +14402,7 @@
       </c>
       <c r="G388" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H388" t="inlineStr">
@@ -14438,7 +14438,7 @@
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H389" t="inlineStr">
@@ -14510,7 +14510,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H391" t="inlineStr">
@@ -14546,7 +14546,7 @@
       </c>
       <c r="G392" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H392" t="inlineStr">
@@ -14582,7 +14582,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -14618,7 +14618,7 @@
       </c>
       <c r="G394" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H394" t="inlineStr">
@@ -14762,7 +14762,7 @@
       </c>
       <c r="G398" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H398" t="inlineStr">
@@ -14798,7 +14798,7 @@
       </c>
       <c r="G399" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H399" t="inlineStr">
@@ -14870,7 +14870,7 @@
       </c>
       <c r="G401" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H401" t="inlineStr">
@@ -14906,7 +14906,7 @@
       </c>
       <c r="G402" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H402" t="inlineStr">
@@ -14942,7 +14942,7 @@
       </c>
       <c r="G403" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H403" t="inlineStr">
@@ -15014,7 +15014,7 @@
       </c>
       <c r="G405" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H405" t="inlineStr">
@@ -15050,7 +15050,7 @@
       </c>
       <c r="G406" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H406" t="inlineStr">
@@ -15122,7 +15122,7 @@
       </c>
       <c r="G408" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H408" t="inlineStr">
@@ -15158,7 +15158,7 @@
       </c>
       <c r="G409" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H409" t="inlineStr">
@@ -15230,7 +15230,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H411" t="inlineStr">
@@ -15410,7 +15410,7 @@
       </c>
       <c r="G416" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H416" t="inlineStr">
@@ -15482,7 +15482,7 @@
       </c>
       <c r="G418" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H418" t="inlineStr">
@@ -15518,7 +15518,7 @@
       </c>
       <c r="G419" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H419" t="inlineStr">
@@ -15554,7 +15554,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H420" t="inlineStr">
@@ -15590,7 +15590,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H421" t="inlineStr">
@@ -15626,7 +15626,7 @@
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H422" t="inlineStr">
@@ -15698,7 +15698,7 @@
       </c>
       <c r="G424" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H424" t="inlineStr">
@@ -15734,7 +15734,7 @@
       </c>
       <c r="G425" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H425" t="inlineStr">
@@ -15770,7 +15770,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H426" t="inlineStr">
@@ -15878,7 +15878,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H429" t="inlineStr">
@@ -15950,7 +15950,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H431" t="inlineStr">
@@ -15986,7 +15986,7 @@
       </c>
       <c r="G432" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H432" t="inlineStr">
@@ -16166,7 +16166,7 @@
       </c>
       <c r="G437" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H437" t="inlineStr">
@@ -16238,7 +16238,7 @@
       </c>
       <c r="G439" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H439" t="inlineStr">
@@ -16274,7 +16274,7 @@
       </c>
       <c r="G440" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Financing Activities (Rule-Interest)</t>
         </is>
       </c>
       <c r="H440" t="inlineStr">
@@ -16310,7 +16310,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H441" t="inlineStr">
@@ -16418,7 +16418,7 @@
       </c>
       <c r="G444" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H444" t="inlineStr">
@@ -16490,7 +16490,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H446" t="inlineStr">
@@ -16526,7 +16526,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H447" t="inlineStr">
@@ -16562,7 +16562,7 @@
       </c>
       <c r="G448" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H448" t="inlineStr">
@@ -16634,7 +16634,7 @@
       </c>
       <c r="G450" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H450" t="inlineStr">
@@ -16706,7 +16706,7 @@
       </c>
       <c r="G452" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H452" t="inlineStr">
@@ -16922,7 +16922,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H458" t="inlineStr">
@@ -16958,7 +16958,7 @@
       </c>
       <c r="G459" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H459" t="inlineStr">
@@ -16994,7 +16994,7 @@
       </c>
       <c r="G460" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H460" t="inlineStr">
@@ -17030,7 +17030,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>Financing Activities (Rule-Finance)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H461" t="inlineStr">
@@ -17102,7 +17102,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H463" t="inlineStr">
@@ -17174,7 +17174,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Operating Activities (Rule-Transport)</t>
         </is>
       </c>
       <c r="H465" t="inlineStr">
@@ -17390,7 +17390,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Operating Activities (Rule-Facility)</t>
         </is>
       </c>
       <c r="H471" t="inlineStr">
@@ -17426,7 +17426,7 @@
       </c>
       <c r="G472" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H472" t="inlineStr">
@@ -17462,7 +17462,7 @@
       </c>
       <c r="G473" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H473" t="inlineStr">
@@ -17498,7 +17498,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H474" t="inlineStr">
@@ -17570,7 +17570,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H476" t="inlineStr">
@@ -17606,7 +17606,7 @@
       </c>
       <c r="G477" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H477" t="inlineStr">
@@ -17642,7 +17642,7 @@
       </c>
       <c r="G478" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H478" t="inlineStr">
@@ -17678,7 +17678,7 @@
       </c>
       <c r="G479" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H479" t="inlineStr">
@@ -17714,7 +17714,7 @@
       </c>
       <c r="G480" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H480" t="inlineStr">
@@ -17750,7 +17750,7 @@
       </c>
       <c r="G481" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H481" t="inlineStr">
@@ -17822,7 +17822,7 @@
       </c>
       <c r="G483" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H483" t="inlineStr">
@@ -17858,7 +17858,7 @@
       </c>
       <c r="G484" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H484" t="inlineStr">
@@ -17894,7 +17894,7 @@
       </c>
       <c r="G485" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H485" t="inlineStr">
@@ -17966,7 +17966,7 @@
       </c>
       <c r="G487" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Vendor)</t>
+          <t>Investing Activities (Rule-Asset)</t>
         </is>
       </c>
       <c r="H487" t="inlineStr">
@@ -18002,7 +18002,7 @@
       </c>
       <c r="G488" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H488" t="inlineStr">
@@ -18038,7 +18038,7 @@
       </c>
       <c r="G489" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H489" t="inlineStr">
@@ -18074,7 +18074,7 @@
       </c>
       <c r="G490" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Utility)</t>
+          <t>Financing Activities (Rule-Debt)</t>
         </is>
       </c>
       <c r="H490" t="inlineStr">
@@ -18110,7 +18110,7 @@
       </c>
       <c r="G491" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H491" t="inlineStr">
@@ -18146,7 +18146,7 @@
       </c>
       <c r="G492" t="inlineStr">
         <is>
-          <t>Operating Activities (Rule-Default)</t>
+          <t>Investing Activities (Rule-Disposal)</t>
         </is>
       </c>
       <c r="H492" t="inlineStr">

</xml_diff>

<commit_message>
changes but no ai
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -526,7 +526,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45659</v>
+        <v>25569.00000000821</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45847</v>
+        <v>25569.00000000774</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45626</v>
+        <v>25569.00000000441</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45697</v>
+        <v>25569.00000000575</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -828,7 +828,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45557</v>
+        <v>25569.00000000527</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -903,7 +903,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45642</v>
+        <v>25569.00000000443</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -978,7 +978,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45747</v>
+        <v>25569.00000000102</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45847</v>
+        <v>25569.00000000064</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45644</v>
+        <v>25569.00000000231</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45702</v>
+        <v>25569.00000000477</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45521</v>
+        <v>25569.0000000056</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45835</v>
+        <v>25569.00000000161</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45774</v>
+        <v>25569.00000000191</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45682</v>
+        <v>25569.00000000419</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45549</v>
+        <v>25569.00000000276</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45631</v>
+        <v>25569.00000000397</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45514</v>
+        <v>25569.00000000213</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45678</v>
+        <v>25569.00000000228</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45713</v>
+        <v>25569.00000001155</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45732</v>
+        <v>25569.00000000572</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45682</v>
+        <v>25569.00000000337</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45768</v>
+        <v>25569.0000000042</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45560</v>
+        <v>25569.00000000303</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45851</v>
+        <v>25569.00000000567</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45639</v>
+        <v>25569.00000001061</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45857</v>
+        <v>25569.00000000787</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45723</v>
+        <v>25569.00000000544</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45844</v>
+        <v>25569.0000000041</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45721</v>
+        <v>25569.00000000205</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45594</v>
+        <v>25569.00000000492</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45793</v>
+        <v>25569.00000000629</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45798</v>
+        <v>25569.00000000337</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45684</v>
+        <v>25569.0000000052</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45640</v>
+        <v>25569.00000000375</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45499</v>
+        <v>25569.00000000111</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45554</v>
+        <v>25569.00000000206</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45748</v>
+        <v>25569.00000000073</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -3311,7 +3311,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45547</v>
+        <v>25569.00000000403</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45511</v>
+        <v>25569.00000001</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45708</v>
+        <v>25569.00000000865</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45763</v>
+        <v>25569.00000000107</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45685</v>
+        <v>25569.00000000037</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45835</v>
+        <v>25569.00000000158</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45800</v>
+        <v>25569.00000000592</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45536</v>
+        <v>25569.00000001112</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -3917,7 +3917,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45701</v>
+        <v>25569.0000000008</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45683</v>
+        <v>25569.00000000255</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -4067,7 +4067,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45597</v>
+        <v>25569.00000000245</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45633</v>
+        <v>25569.00000000583</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -4217,7 +4217,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45714</v>
+        <v>25569.00000000425</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -4292,7 +4292,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45841</v>
+        <v>25569.00000000294</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -4367,7 +4367,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45539</v>
+        <v>25569.00000000438</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45725</v>
+        <v>25569.00000000231</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45527</v>
+        <v>25569.00000000961</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45763</v>
+        <v>25569.00000000153</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -4667,7 +4667,7 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45758</v>
+        <v>25569.00000001242</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -4742,7 +4742,7 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45526</v>
+        <v>25569.0000000045</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -4817,7 +4817,7 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45700</v>
+        <v>25569.00000000535</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -4894,7 +4894,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45778</v>
+        <v>25569.00000000251</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45713</v>
+        <v>25569.00000000139</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -5044,7 +5044,7 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45729</v>
+        <v>25569.00000000133</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -5119,7 +5119,7 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45500</v>
+        <v>25569.0000000044</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -5194,7 +5194,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45813</v>
+        <v>25569.00000000473</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -5269,7 +5269,7 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45625</v>
+        <v>25569.00000000513</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -5344,7 +5344,7 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45705</v>
+        <v>25569.00000000059</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -5419,7 +5419,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45859</v>
+        <v>25569.00000000207</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -5494,7 +5494,7 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45527</v>
+        <v>25569.00000000222</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -5569,7 +5569,7 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45600</v>
+        <v>25569.00000000397</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>45682</v>
+        <v>25569.00000000319</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -5719,7 +5719,7 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>45499</v>
+        <v>25569.00000000522</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -5794,7 +5794,7 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>45524</v>
+        <v>25569.00000000324</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -5869,7 +5869,7 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>45609</v>
+        <v>25569.00000000456</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -5944,7 +5944,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>45613</v>
+        <v>25569.00000000566</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -6019,7 +6019,7 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>45574</v>
+        <v>25569.00000000083</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -6096,7 +6096,7 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>45772</v>
+        <v>25569.00000000824</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -6171,7 +6171,7 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>45591</v>
+        <v>25569.00000000474</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -6246,7 +6246,7 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>45736</v>
+        <v>25569.00000000147</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -6321,7 +6321,7 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>45808</v>
+        <v>25569.00000000785</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -6396,7 +6396,7 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>45558</v>
+        <v>25569.00000000342</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -6473,7 +6473,7 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>45666</v>
+        <v>25569.00000000336</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -6550,7 +6550,7 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>45509</v>
+        <v>25569.00000000221</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -6627,7 +6627,7 @@
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>45806</v>
+        <v>25569.00000000287</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -6702,7 +6702,7 @@
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>45550</v>
+        <v>25569.00000000135</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -6777,7 +6777,7 @@
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>45822</v>
+        <v>25569.00000000501</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -6852,7 +6852,7 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>45823</v>
+        <v>25569.00000000161</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -6929,7 +6929,7 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>45605</v>
+        <v>25569.00000000081</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -7004,7 +7004,7 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>45755</v>
+        <v>25569.00000000514</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -7079,7 +7079,7 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>45575</v>
+        <v>25569.00000000235</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -7154,7 +7154,7 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>45700</v>
+        <v>25569.00000000088</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -7229,7 +7229,7 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>45629</v>
+        <v>25569.00000000497</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -7304,7 +7304,7 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>45829</v>
+        <v>25569.00000000366</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -7379,7 +7379,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>45672</v>
+        <v>25569.00000000427</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -7454,7 +7454,7 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>45585</v>
+        <v>25569.00000000445</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -7529,7 +7529,7 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>45710</v>
+        <v>25569.00000000189</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -7604,7 +7604,7 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>45592</v>
+        <v>25569.00000000065</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -7679,7 +7679,7 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>45819</v>
+        <v>25569.00000000342</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -7754,7 +7754,7 @@
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>45698</v>
+        <v>25569.00000000264</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -7829,7 +7829,7 @@
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>45720</v>
+        <v>25569.00000000106</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -7904,7 +7904,7 @@
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>45634</v>
+        <v>25569.00000000334</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -7979,7 +7979,7 @@
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>45543</v>
+        <v>25569.00000000162</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -8056,7 +8056,7 @@
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>45718</v>
+        <v>25569.00000000363</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -8131,7 +8131,7 @@
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>45613</v>
+        <v>25569.00000000222</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -8206,7 +8206,7 @@
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>45745</v>
+        <v>25569.00000000186</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -8281,7 +8281,7 @@
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>45582</v>
+        <v>25569.00000000202</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -8358,7 +8358,7 @@
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>45796</v>
+        <v>25569.00000000448</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>45580</v>
+        <v>25569.00000000256</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -8508,7 +8508,7 @@
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>45601</v>
+        <v>25569.00000000346</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -8583,7 +8583,7 @@
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>45576</v>
+        <v>25569.00000000028</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -8660,7 +8660,7 @@
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>45585</v>
+        <v>25569.00000000912</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -8735,7 +8735,7 @@
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>45856</v>
+        <v>25569.00000000375</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -8810,7 +8810,7 @@
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>45840</v>
+        <v>25569.00000001012</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -8885,7 +8885,7 @@
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>45654</v>
+        <v>25569.00000000035</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -8960,7 +8960,7 @@
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>45861</v>
+        <v>25569.0000000057</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -9035,7 +9035,7 @@
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>45847</v>
+        <v>25569.00000000376</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -9110,7 +9110,7 @@
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>45729</v>
+        <v>25569.00000000294</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -9185,7 +9185,7 @@
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>45660</v>
+        <v>25569.00000000091</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -9260,7 +9260,7 @@
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>45502</v>
+        <v>25569.00000000255</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -9337,7 +9337,7 @@
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>45654</v>
+        <v>25569.00000000151</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -9414,7 +9414,7 @@
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>45604</v>
+        <v>25569.00000000244</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -9489,7 +9489,7 @@
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>45561</v>
+        <v>25569.00000000185</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -9564,7 +9564,7 @@
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>45577</v>
+        <v>25569.00000001044</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -9639,7 +9639,7 @@
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>45648</v>
+        <v>25569.00000000327</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -9716,7 +9716,7 @@
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>45608</v>
+        <v>25569.00000000073</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -9793,7 +9793,7 @@
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>45767</v>
+        <v>25569.0000000017</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -9868,7 +9868,7 @@
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>45539</v>
+        <v>25569.00000000422</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -9943,7 +9943,7 @@
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>45537</v>
+        <v>25569.00000000245</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -10018,7 +10018,7 @@
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>45571</v>
+        <v>25569.00000000805</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -10093,7 +10093,7 @@
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>45545</v>
+        <v>25569.00000000558</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -10168,7 +10168,7 @@
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>45859</v>
+        <v>25569.00000000296</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -10245,7 +10245,7 @@
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>45583</v>
+        <v>25569.00000000109</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -10320,7 +10320,7 @@
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>45504</v>
+        <v>25569.000000001</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -10395,7 +10395,7 @@
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>45835</v>
+        <v>25569.00000000805</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -10470,7 +10470,7 @@
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>45596</v>
+        <v>25569.0000000057</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -10547,7 +10547,7 @@
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>45673</v>
+        <v>25569.0000000102</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -10622,7 +10622,7 @@
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>45768</v>
+        <v>25569.00000000111</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -10697,7 +10697,7 @@
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>45503</v>
+        <v>25569.00000001111</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -10772,7 +10772,7 @@
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>45762</v>
+        <v>25569.00000000231</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -10847,7 +10847,7 @@
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>45656</v>
+        <v>25569.00000000191</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -10922,7 +10922,7 @@
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>45826</v>
+        <v>25569.00000000072</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -10999,7 +10999,7 @@
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>45802</v>
+        <v>25569.0000000051</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -11074,7 +11074,7 @@
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>45764</v>
+        <v>25569.00000000522</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -11149,7 +11149,7 @@
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>45578</v>
+        <v>25569.00000000232</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -11224,7 +11224,7 @@
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
-        <v>45666</v>
+        <v>25569.00000001046</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -11299,7 +11299,7 @@
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
-        <v>45668</v>
+        <v>25569.00000000467</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -11374,7 +11374,7 @@
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
-        <v>45781</v>
+        <v>25569.00000000154</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -11449,7 +11449,7 @@
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
-        <v>45806</v>
+        <v>25569.00000000396</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -11524,7 +11524,7 @@
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
-        <v>45572</v>
+        <v>25569.0000000012</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -11599,7 +11599,7 @@
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
-        <v>45534</v>
+        <v>25569.00000000381</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -11674,7 +11674,7 @@
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
-        <v>45837</v>
+        <v>25569.00000000257</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -11749,7 +11749,7 @@
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
-        <v>45817</v>
+        <v>25569.0000000103</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -11824,7 +11824,7 @@
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
-        <v>45847</v>
+        <v>25569.0000000048</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -11899,7 +11899,7 @@
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
-        <v>45557</v>
+        <v>25569.00000000238</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -11974,7 +11974,7 @@
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
-        <v>45516</v>
+        <v>25569.00000000418</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -12049,7 +12049,7 @@
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
-        <v>45502</v>
+        <v>25569.00000000084</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -12126,7 +12126,7 @@
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
-        <v>45685</v>
+        <v>25569.00000000174</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -12203,7 +12203,7 @@
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
-        <v>45727</v>
+        <v>25569.00000000373</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -12278,7 +12278,7 @@
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
-        <v>45605</v>
+        <v>25569.00000000117</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -12353,7 +12353,7 @@
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
-        <v>45630</v>
+        <v>25569.00000000065</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -12428,7 +12428,7 @@
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
-        <v>45636</v>
+        <v>25569.00000000123</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -12503,7 +12503,7 @@
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
-        <v>45627</v>
+        <v>25569.00000000089</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -12578,7 +12578,7 @@
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
-        <v>45628</v>
+        <v>25569.0000000081</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -12653,7 +12653,7 @@
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
-        <v>45661</v>
+        <v>25569.00000000231</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -12728,7 +12728,7 @@
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
-        <v>45646</v>
+        <v>25569.00000000307</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -12803,7 +12803,7 @@
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
-        <v>45663</v>
+        <v>25569.00000000667</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -12878,7 +12878,7 @@
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
-        <v>45789</v>
+        <v>25569.00000000325</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -12953,7 +12953,7 @@
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
-        <v>45779</v>
+        <v>25569.00000000572</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -13028,7 +13028,7 @@
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
-        <v>45600</v>
+        <v>25569.0000000011</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -13103,7 +13103,7 @@
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
-        <v>45712</v>
+        <v>25569.00000000523</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -13178,7 +13178,7 @@
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
-        <v>45822</v>
+        <v>25569.00000000543</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -13253,7 +13253,7 @@
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
-        <v>45660</v>
+        <v>25569.00000000185</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -13328,7 +13328,7 @@
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
-        <v>45724</v>
+        <v>25569.00000000429</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -13403,7 +13403,7 @@
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
-        <v>45534</v>
+        <v>25569.00000000077</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -13480,7 +13480,7 @@
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
-        <v>45793</v>
+        <v>25569.00000000084</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -13557,7 +13557,7 @@
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
-        <v>45666</v>
+        <v>25569.00000000119</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -13632,7 +13632,7 @@
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
-        <v>45651</v>
+        <v>25569.00000000131</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -13707,7 +13707,7 @@
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
-        <v>45667</v>
+        <v>25569.00000000194</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -13782,7 +13782,7 @@
     </row>
     <row r="178">
       <c r="A178" s="2" t="n">
-        <v>45553</v>
+        <v>25569.00000000159</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -13857,7 +13857,7 @@
     </row>
     <row r="179">
       <c r="A179" s="2" t="n">
-        <v>45662</v>
+        <v>25569.00000000066</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
@@ -13932,7 +13932,7 @@
     </row>
     <row r="180">
       <c r="A180" s="2" t="n">
-        <v>45579</v>
+        <v>25569.0000000033</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
@@ -14007,7 +14007,7 @@
     </row>
     <row r="181">
       <c r="A181" s="2" t="n">
-        <v>45808</v>
+        <v>25569.00000000602</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
@@ -14082,7 +14082,7 @@
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45628</v>
+        <v>25569.00000000227</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
@@ -14157,7 +14157,7 @@
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
-        <v>45757</v>
+        <v>25569.00000000194</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
@@ -14232,7 +14232,7 @@
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
-        <v>45760</v>
+        <v>25569.00000000152</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
@@ -14307,7 +14307,7 @@
     </row>
     <row r="185">
       <c r="A185" s="2" t="n">
-        <v>45614</v>
+        <v>25569.0000000012</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
@@ -14382,7 +14382,7 @@
     </row>
     <row r="186">
       <c r="A186" s="2" t="n">
-        <v>45704</v>
+        <v>25569.00000000389</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
@@ -14457,7 +14457,7 @@
     </row>
     <row r="187">
       <c r="A187" s="2" t="n">
-        <v>45775</v>
+        <v>25569.00000000905</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
@@ -14532,7 +14532,7 @@
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
-        <v>45699</v>
+        <v>25569.00000000441</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
@@ -14607,7 +14607,7 @@
     </row>
     <row r="189">
       <c r="A189" s="2" t="n">
-        <v>45647</v>
+        <v>25569.0000000054</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
@@ -14682,7 +14682,7 @@
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
-        <v>45825</v>
+        <v>25569.00000000558</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
@@ -14757,7 +14757,7 @@
     </row>
     <row r="191">
       <c r="A191" s="2" t="n">
-        <v>45749</v>
+        <v>25569.00000000399</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
@@ -14832,7 +14832,7 @@
     </row>
     <row r="192">
       <c r="A192" s="2" t="n">
-        <v>45764</v>
+        <v>25569.0000000018</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
@@ -14907,7 +14907,7 @@
     </row>
     <row r="193">
       <c r="A193" s="2" t="n">
-        <v>45596</v>
+        <v>25569.00000000434</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
@@ -14982,7 +14982,7 @@
     </row>
     <row r="194">
       <c r="A194" s="2" t="n">
-        <v>45754</v>
+        <v>25569.00000000492</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
@@ -15057,7 +15057,7 @@
     </row>
     <row r="195">
       <c r="A195" s="2" t="n">
-        <v>45598</v>
+        <v>25569.00000000087</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
@@ -15132,7 +15132,7 @@
     </row>
     <row r="196">
       <c r="A196" s="2" t="n">
-        <v>45782</v>
+        <v>25569.00000001307</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
@@ -15207,7 +15207,7 @@
     </row>
     <row r="197">
       <c r="A197" s="2" t="n">
-        <v>45507</v>
+        <v>25569.00000000495</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
@@ -15284,7 +15284,7 @@
     </row>
     <row r="198">
       <c r="A198" s="2" t="n">
-        <v>45824</v>
+        <v>25569.00000000221</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
@@ -15359,7 +15359,7 @@
     </row>
     <row r="199">
       <c r="A199" s="2" t="n">
-        <v>45847</v>
+        <v>25569.00000000264</v>
       </c>
       <c r="B199" t="inlineStr">
         <is>
@@ -15434,7 +15434,7 @@
     </row>
     <row r="200">
       <c r="A200" s="2" t="n">
-        <v>45772</v>
+        <v>25569.00000000315</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
@@ -15511,7 +15511,7 @@
     </row>
     <row r="201">
       <c r="A201" s="2" t="n">
-        <v>45833</v>
+        <v>25569.0000000033</v>
       </c>
       <c r="B201" t="inlineStr">
         <is>
@@ -15586,7 +15586,7 @@
     </row>
     <row r="202">
       <c r="A202" s="2" t="n">
-        <v>45813</v>
+        <v>25569.00000000075</v>
       </c>
       <c r="B202" t="inlineStr">
         <is>
@@ -15661,7 +15661,7 @@
     </row>
     <row r="203">
       <c r="A203" s="2" t="n">
-        <v>45626</v>
+        <v>25569.00000000072</v>
       </c>
       <c r="B203" t="inlineStr">
         <is>
@@ -15736,7 +15736,7 @@
     </row>
     <row r="204">
       <c r="A204" s="2" t="n">
-        <v>45859</v>
+        <v>25569.00000000276</v>
       </c>
       <c r="B204" t="inlineStr">
         <is>
@@ -15811,7 +15811,7 @@
     </row>
     <row r="205">
       <c r="A205" s="2" t="n">
-        <v>45513</v>
+        <v>25569.00000000667</v>
       </c>
       <c r="B205" t="inlineStr">
         <is>
@@ -15886,7 +15886,7 @@
     </row>
     <row r="206">
       <c r="A206" s="2" t="n">
-        <v>45554</v>
+        <v>25569.00000000151</v>
       </c>
       <c r="B206" t="inlineStr">
         <is>
@@ -15961,7 +15961,7 @@
     </row>
     <row r="207">
       <c r="A207" s="2" t="n">
-        <v>45570</v>
+        <v>25569.00000000046</v>
       </c>
       <c r="B207" t="inlineStr">
         <is>
@@ -16038,7 +16038,7 @@
     </row>
     <row r="208">
       <c r="A208" s="2" t="n">
-        <v>45550</v>
+        <v>25569.00000000081</v>
       </c>
       <c r="B208" t="inlineStr">
         <is>
@@ -16113,7 +16113,7 @@
     </row>
     <row r="209">
       <c r="A209" s="2" t="n">
-        <v>45632</v>
+        <v>25569.0000000031</v>
       </c>
       <c r="B209" t="inlineStr">
         <is>
@@ -16188,7 +16188,7 @@
     </row>
     <row r="210">
       <c r="A210" s="2" t="n">
-        <v>45645</v>
+        <v>25569.00000000178</v>
       </c>
       <c r="B210" t="inlineStr">
         <is>
@@ -16263,7 +16263,7 @@
     </row>
     <row r="211">
       <c r="A211" s="2" t="n">
-        <v>45751</v>
+        <v>25569.00000000294</v>
       </c>
       <c r="B211" t="inlineStr">
         <is>
@@ -16338,7 +16338,7 @@
     </row>
     <row r="212">
       <c r="A212" s="2" t="n">
-        <v>45725</v>
+        <v>25569.0000000006</v>
       </c>
       <c r="B212" t="inlineStr">
         <is>
@@ -16415,7 +16415,7 @@
     </row>
     <row r="213">
       <c r="A213" s="2" t="n">
-        <v>45679</v>
+        <v>25569.00000000459</v>
       </c>
       <c r="B213" t="inlineStr">
         <is>
@@ -16490,7 +16490,7 @@
     </row>
     <row r="214">
       <c r="A214" s="2" t="n">
-        <v>45740</v>
+        <v>25569.00000000296</v>
       </c>
       <c r="B214" t="inlineStr">
         <is>
@@ -16565,7 +16565,7 @@
     </row>
     <row r="215">
       <c r="A215" s="2" t="n">
-        <v>45579</v>
+        <v>25569.00000000333</v>
       </c>
       <c r="B215" t="inlineStr">
         <is>
@@ -16640,7 +16640,7 @@
     </row>
     <row r="216">
       <c r="A216" s="2" t="n">
-        <v>45529</v>
+        <v>25569.00000000149</v>
       </c>
       <c r="B216" t="inlineStr">
         <is>
@@ -16715,7 +16715,7 @@
     </row>
     <row r="217">
       <c r="A217" s="2" t="n">
-        <v>45727</v>
+        <v>25569.00000000397</v>
       </c>
       <c r="B217" t="inlineStr">
         <is>
@@ -16790,7 +16790,7 @@
     </row>
     <row r="218">
       <c r="A218" s="2" t="n">
-        <v>45530</v>
+        <v>25569.0000000022</v>
       </c>
       <c r="B218" t="inlineStr">
         <is>
@@ -16865,7 +16865,7 @@
     </row>
     <row r="219">
       <c r="A219" s="2" t="n">
-        <v>45844</v>
+        <v>25569.00000000097</v>
       </c>
       <c r="B219" t="inlineStr">
         <is>
@@ -16940,7 +16940,7 @@
     </row>
     <row r="220">
       <c r="A220" s="2" t="n">
-        <v>45689</v>
+        <v>25569.00000001175</v>
       </c>
       <c r="B220" t="inlineStr">
         <is>
@@ -17015,7 +17015,7 @@
     </row>
     <row r="221">
       <c r="A221" s="2" t="n">
-        <v>45542</v>
+        <v>25569.00000000969</v>
       </c>
       <c r="B221" t="inlineStr">
         <is>
@@ -17090,7 +17090,7 @@
     </row>
     <row r="222">
       <c r="A222" s="2" t="n">
-        <v>45843</v>
+        <v>25569.00000001155</v>
       </c>
       <c r="B222" t="inlineStr">
         <is>
@@ -17165,7 +17165,7 @@
     </row>
     <row r="223">
       <c r="A223" s="2" t="n">
-        <v>45852</v>
+        <v>25569.0000000036</v>
       </c>
       <c r="B223" t="inlineStr">
         <is>
@@ -17240,7 +17240,7 @@
     </row>
     <row r="224">
       <c r="A224" s="2" t="n">
-        <v>45787</v>
+        <v>25569.00000000162</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
@@ -17315,7 +17315,7 @@
     </row>
     <row r="225">
       <c r="A225" s="2" t="n">
-        <v>45578</v>
+        <v>25569.00000000067</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
@@ -17390,7 +17390,7 @@
     </row>
     <row r="226">
       <c r="A226" s="2" t="n">
-        <v>45709</v>
+        <v>25569.00000000184</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
@@ -17465,7 +17465,7 @@
     </row>
     <row r="227">
       <c r="A227" s="2" t="n">
-        <v>45626</v>
+        <v>25569.00000000204</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
@@ -17540,7 +17540,7 @@
     </row>
     <row r="228">
       <c r="A228" s="2" t="n">
-        <v>45534</v>
+        <v>25569.00000000115</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
@@ -17615,7 +17615,7 @@
     </row>
     <row r="229">
       <c r="A229" s="2" t="n">
-        <v>45844</v>
+        <v>25569.00000000492</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
@@ -17692,7 +17692,7 @@
     </row>
     <row r="230">
       <c r="A230" s="2" t="n">
-        <v>45756</v>
+        <v>25569.00000000148</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
@@ -17767,7 +17767,7 @@
     </row>
     <row r="231">
       <c r="A231" s="2" t="n">
-        <v>45851</v>
+        <v>25569.00000000594</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
@@ -17842,7 +17842,7 @@
     </row>
     <row r="232">
       <c r="A232" s="2" t="n">
-        <v>45793</v>
+        <v>25569.00000000561</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
@@ -17917,7 +17917,7 @@
     </row>
     <row r="233">
       <c r="A233" s="2" t="n">
-        <v>45750</v>
+        <v>25569.00000000436</v>
       </c>
       <c r="B233" t="inlineStr">
         <is>
@@ -17992,7 +17992,7 @@
     </row>
     <row r="234">
       <c r="A234" s="2" t="n">
-        <v>45695</v>
+        <v>25569.00000000085</v>
       </c>
       <c r="B234" t="inlineStr">
         <is>
@@ -18067,7 +18067,7 @@
     </row>
     <row r="235">
       <c r="A235" s="2" t="n">
-        <v>45538</v>
+        <v>25569.00000000602</v>
       </c>
       <c r="B235" t="inlineStr">
         <is>
@@ -18144,7 +18144,7 @@
     </row>
     <row r="236">
       <c r="A236" s="2" t="n">
-        <v>45671</v>
+        <v>25569.0000000021</v>
       </c>
       <c r="B236" t="inlineStr">
         <is>
@@ -18219,7 +18219,7 @@
     </row>
     <row r="237">
       <c r="A237" s="2" t="n">
-        <v>45628</v>
+        <v>25569.00000000879</v>
       </c>
       <c r="B237" t="inlineStr">
         <is>
@@ -18294,7 +18294,7 @@
     </row>
     <row r="238">
       <c r="A238" s="2" t="n">
-        <v>45580</v>
+        <v>25569.00000000221</v>
       </c>
       <c r="B238" t="inlineStr">
         <is>
@@ -18369,7 +18369,7 @@
     </row>
     <row r="239">
       <c r="A239" s="2" t="n">
-        <v>45687</v>
+        <v>25569.00000000759</v>
       </c>
       <c r="B239" t="inlineStr">
         <is>
@@ -18444,7 +18444,7 @@
     </row>
     <row r="240">
       <c r="A240" s="2" t="n">
-        <v>45500</v>
+        <v>25569.00000000112</v>
       </c>
       <c r="B240" t="inlineStr">
         <is>
@@ -18519,7 +18519,7 @@
     </row>
     <row r="241">
       <c r="A241" s="2" t="n">
-        <v>45842</v>
+        <v>25569.0000000005</v>
       </c>
       <c r="B241" t="inlineStr">
         <is>
@@ -18594,7 +18594,7 @@
     </row>
     <row r="242">
       <c r="A242" s="2" t="n">
-        <v>45527</v>
+        <v>25569.00000000476</v>
       </c>
       <c r="B242" t="inlineStr">
         <is>
@@ -18669,7 +18669,7 @@
     </row>
     <row r="243">
       <c r="A243" s="2" t="n">
-        <v>45778</v>
+        <v>25569.00000000156</v>
       </c>
       <c r="B243" t="inlineStr">
         <is>
@@ -18744,7 +18744,7 @@
     </row>
     <row r="244">
       <c r="A244" s="2" t="n">
-        <v>45582</v>
+        <v>25569.00000000471</v>
       </c>
       <c r="B244" t="inlineStr">
         <is>
@@ -18819,7 +18819,7 @@
     </row>
     <row r="245">
       <c r="A245" s="2" t="n">
-        <v>45784</v>
+        <v>25569.00000000043</v>
       </c>
       <c r="B245" t="inlineStr">
         <is>
@@ -18894,7 +18894,7 @@
     </row>
     <row r="246">
       <c r="A246" s="2" t="n">
-        <v>45775</v>
+        <v>25569.00000000169</v>
       </c>
       <c r="B246" t="inlineStr">
         <is>
@@ -18969,7 +18969,7 @@
     </row>
     <row r="247">
       <c r="A247" s="2" t="n">
-        <v>45599</v>
+        <v>25569.00000000429</v>
       </c>
       <c r="B247" t="inlineStr">
         <is>
@@ -19044,7 +19044,7 @@
     </row>
     <row r="248">
       <c r="A248" s="2" t="n">
-        <v>45597</v>
+        <v>25569.00000000167</v>
       </c>
       <c r="B248" t="inlineStr">
         <is>
@@ -19119,7 +19119,7 @@
     </row>
     <row r="249">
       <c r="A249" s="2" t="n">
-        <v>45803</v>
+        <v>25569.000000009</v>
       </c>
       <c r="B249" t="inlineStr">
         <is>
@@ -19194,7 +19194,7 @@
     </row>
     <row r="250">
       <c r="A250" s="2" t="n">
-        <v>45828</v>
+        <v>25569.00000000107</v>
       </c>
       <c r="B250" t="inlineStr">
         <is>
@@ -19269,7 +19269,7 @@
     </row>
     <row r="251">
       <c r="A251" s="2" t="n">
-        <v>45826</v>
+        <v>25569.00000000112</v>
       </c>
       <c r="B251" t="inlineStr">
         <is>
@@ -19344,7 +19344,7 @@
     </row>
     <row r="252">
       <c r="A252" s="2" t="n">
-        <v>45661</v>
+        <v>25569.00000000053</v>
       </c>
       <c r="B252" t="inlineStr">
         <is>
@@ -19421,7 +19421,7 @@
     </row>
     <row r="253">
       <c r="A253" s="2" t="n">
-        <v>45568</v>
+        <v>25569.00000000203</v>
       </c>
       <c r="B253" t="inlineStr">
         <is>
@@ -19496,7 +19496,7 @@
     </row>
     <row r="254">
       <c r="A254" s="2" t="n">
-        <v>45552</v>
+        <v>25569.00000000873</v>
       </c>
       <c r="B254" t="inlineStr">
         <is>
@@ -19571,7 +19571,7 @@
     </row>
     <row r="255">
       <c r="A255" s="2" t="n">
-        <v>45591</v>
+        <v>25569.00000000082</v>
       </c>
       <c r="B255" t="inlineStr">
         <is>
@@ -19646,7 +19646,7 @@
     </row>
     <row r="256">
       <c r="A256" s="2" t="n">
-        <v>45833</v>
+        <v>25569.0000000022</v>
       </c>
       <c r="B256" t="inlineStr">
         <is>
@@ -19721,7 +19721,7 @@
     </row>
     <row r="257">
       <c r="A257" s="2" t="n">
-        <v>45643</v>
+        <v>25569.00000000133</v>
       </c>
       <c r="B257" t="inlineStr">
         <is>
@@ -19796,7 +19796,7 @@
     </row>
     <row r="258">
       <c r="A258" s="2" t="n">
-        <v>45787</v>
+        <v>25569.00000000218</v>
       </c>
       <c r="B258" t="inlineStr">
         <is>
@@ -19871,7 +19871,7 @@
     </row>
     <row r="259">
       <c r="A259" s="2" t="n">
-        <v>45817</v>
+        <v>25569.0000000009</v>
       </c>
       <c r="B259" t="inlineStr">
         <is>
@@ -19946,7 +19946,7 @@
     </row>
     <row r="260">
       <c r="A260" s="2" t="n">
-        <v>45743</v>
+        <v>25569.00000000521</v>
       </c>
       <c r="B260" t="inlineStr">
         <is>
@@ -20021,7 +20021,7 @@
     </row>
     <row r="261">
       <c r="A261" s="2" t="n">
-        <v>45529</v>
+        <v>25569.00000000415</v>
       </c>
       <c r="B261" t="inlineStr">
         <is>
@@ -20096,7 +20096,7 @@
     </row>
     <row r="262">
       <c r="A262" s="2" t="n">
-        <v>45552</v>
+        <v>25569.00000000304</v>
       </c>
       <c r="B262" t="inlineStr">
         <is>
@@ -20171,7 +20171,7 @@
     </row>
     <row r="263">
       <c r="A263" s="2" t="n">
-        <v>45675</v>
+        <v>25569.00000000109</v>
       </c>
       <c r="B263" t="inlineStr">
         <is>
@@ -20246,7 +20246,7 @@
     </row>
     <row r="264">
       <c r="A264" s="2" t="n">
-        <v>45500</v>
+        <v>25569.00000000145</v>
       </c>
       <c r="B264" t="inlineStr">
         <is>
@@ -20321,7 +20321,7 @@
     </row>
     <row r="265">
       <c r="A265" s="2" t="n">
-        <v>45688</v>
+        <v>25569.00000000229</v>
       </c>
       <c r="B265" t="inlineStr">
         <is>
@@ -20396,7 +20396,7 @@
     </row>
     <row r="266">
       <c r="A266" s="2" t="n">
-        <v>45758</v>
+        <v>25569.00000000492</v>
       </c>
       <c r="B266" t="inlineStr">
         <is>
@@ -20471,7 +20471,7 @@
     </row>
     <row r="267">
       <c r="A267" s="2" t="n">
-        <v>45571</v>
+        <v>25569.00000000066</v>
       </c>
       <c r="B267" t="inlineStr">
         <is>
@@ -20546,7 +20546,7 @@
     </row>
     <row r="268">
       <c r="A268" s="2" t="n">
-        <v>45634</v>
+        <v>25569.00000000515</v>
       </c>
       <c r="B268" t="inlineStr">
         <is>
@@ -20621,7 +20621,7 @@
     </row>
     <row r="269">
       <c r="A269" s="2" t="n">
-        <v>45737</v>
+        <v>25569.00000000098</v>
       </c>
       <c r="B269" t="inlineStr">
         <is>
@@ -20696,7 +20696,7 @@
     </row>
     <row r="270">
       <c r="A270" s="2" t="n">
-        <v>45685</v>
+        <v>25569.00000000493</v>
       </c>
       <c r="B270" t="inlineStr">
         <is>
@@ -20771,7 +20771,7 @@
     </row>
     <row r="271">
       <c r="A271" s="2" t="n">
-        <v>45579</v>
+        <v>25569.00000000538</v>
       </c>
       <c r="B271" t="inlineStr">
         <is>
@@ -20848,7 +20848,7 @@
     </row>
     <row r="272">
       <c r="A272" s="2" t="n">
-        <v>45539</v>
+        <v>25569.00000002152</v>
       </c>
       <c r="B272" t="inlineStr">
         <is>
@@ -20923,7 +20923,7 @@
     </row>
     <row r="273">
       <c r="A273" s="2" t="n">
-        <v>45747</v>
+        <v>25569.00000000522</v>
       </c>
       <c r="B273" t="inlineStr">
         <is>
@@ -20998,7 +20998,7 @@
     </row>
     <row r="274">
       <c r="A274" s="2" t="n">
-        <v>45829</v>
+        <v>25569.00000000244</v>
       </c>
       <c r="B274" t="inlineStr">
         <is>
@@ -21073,7 +21073,7 @@
     </row>
     <row r="275">
       <c r="A275" s="2" t="n">
-        <v>45581</v>
+        <v>25569.00000000268</v>
       </c>
       <c r="B275" t="inlineStr">
         <is>
@@ -21148,7 +21148,7 @@
     </row>
     <row r="276">
       <c r="A276" s="2" t="n">
-        <v>45644</v>
+        <v>25569.00000000228</v>
       </c>
       <c r="B276" t="inlineStr">
         <is>
@@ -21223,7 +21223,7 @@
     </row>
     <row r="277">
       <c r="A277" s="2" t="n">
-        <v>45798</v>
+        <v>25569.00000000203</v>
       </c>
       <c r="B277" t="inlineStr">
         <is>
@@ -21300,7 +21300,7 @@
     </row>
     <row r="278">
       <c r="A278" s="2" t="n">
-        <v>45571</v>
+        <v>25569.00000000455</v>
       </c>
       <c r="B278" t="inlineStr">
         <is>
@@ -21375,7 +21375,7 @@
     </row>
     <row r="279">
       <c r="A279" s="2" t="n">
-        <v>45660</v>
+        <v>25569.00000000436</v>
       </c>
       <c r="B279" t="inlineStr">
         <is>
@@ -21450,7 +21450,7 @@
     </row>
     <row r="280">
       <c r="A280" s="2" t="n">
-        <v>45828</v>
+        <v>25569.00000000549</v>
       </c>
       <c r="B280" t="inlineStr">
         <is>
@@ -21525,7 +21525,7 @@
     </row>
     <row r="281">
       <c r="A281" s="2" t="n">
-        <v>45631</v>
+        <v>25569.00000000074</v>
       </c>
       <c r="B281" t="inlineStr">
         <is>
@@ -21602,7 +21602,7 @@
     </row>
     <row r="282">
       <c r="A282" s="2" t="n">
-        <v>45714</v>
+        <v>25569.00000000431</v>
       </c>
       <c r="B282" t="inlineStr">
         <is>
@@ -21677,7 +21677,7 @@
     </row>
     <row r="283">
       <c r="A283" s="2" t="n">
-        <v>45718</v>
+        <v>25569.00000000184</v>
       </c>
       <c r="B283" t="inlineStr">
         <is>
@@ -21754,7 +21754,7 @@
     </row>
     <row r="284">
       <c r="A284" s="2" t="n">
-        <v>45541</v>
+        <v>25569.00000000276</v>
       </c>
       <c r="B284" t="inlineStr">
         <is>
@@ -21831,7 +21831,7 @@
     </row>
     <row r="285">
       <c r="A285" s="2" t="n">
-        <v>45738</v>
+        <v>25569.0000000003</v>
       </c>
       <c r="B285" t="inlineStr">
         <is>
@@ -21906,7 +21906,7 @@
     </row>
     <row r="286">
       <c r="A286" s="2" t="n">
-        <v>45768</v>
+        <v>25569.00000000199</v>
       </c>
       <c r="B286" t="inlineStr">
         <is>
@@ -21981,7 +21981,7 @@
     </row>
     <row r="287">
       <c r="A287" s="2" t="n">
-        <v>45831</v>
+        <v>25569.00000000061</v>
       </c>
       <c r="B287" t="inlineStr">
         <is>
@@ -22056,7 +22056,7 @@
     </row>
     <row r="288">
       <c r="A288" s="2" t="n">
-        <v>45545</v>
+        <v>25569.00000000013</v>
       </c>
       <c r="B288" t="inlineStr">
         <is>
@@ -22133,7 +22133,7 @@
     </row>
     <row r="289">
       <c r="A289" s="2" t="n">
-        <v>45597</v>
+        <v>25569.00000000409</v>
       </c>
       <c r="B289" t="inlineStr">
         <is>
@@ -22208,7 +22208,7 @@
     </row>
     <row r="290">
       <c r="A290" s="2" t="n">
-        <v>45839</v>
+        <v>25569.00000000126</v>
       </c>
       <c r="B290" t="inlineStr">
         <is>
@@ -22283,7 +22283,7 @@
     </row>
     <row r="291">
       <c r="A291" s="2" t="n">
-        <v>45733</v>
+        <v>25569.0000000218</v>
       </c>
       <c r="B291" t="inlineStr">
         <is>
@@ -22358,7 +22358,7 @@
     </row>
     <row r="292">
       <c r="A292" s="2" t="n">
-        <v>45738</v>
+        <v>25569.00000000511</v>
       </c>
       <c r="B292" t="inlineStr">
         <is>
@@ -22433,7 +22433,7 @@
     </row>
     <row r="293">
       <c r="A293" s="2" t="n">
-        <v>45608</v>
+        <v>25569.00000000117</v>
       </c>
       <c r="B293" t="inlineStr">
         <is>
@@ -22510,7 +22510,7 @@
     </row>
     <row r="294">
       <c r="A294" s="2" t="n">
-        <v>45830</v>
+        <v>25569.00000000049</v>
       </c>
       <c r="B294" t="inlineStr">
         <is>
@@ -22585,7 +22585,7 @@
     </row>
     <row r="295">
       <c r="A295" s="2" t="n">
-        <v>45787</v>
+        <v>25569.00000000273</v>
       </c>
       <c r="B295" t="inlineStr">
         <is>
@@ -22660,7 +22660,7 @@
     </row>
     <row r="296">
       <c r="A296" s="2" t="n">
-        <v>45666</v>
+        <v>25569.00000000102</v>
       </c>
       <c r="B296" t="inlineStr">
         <is>
@@ -22735,7 +22735,7 @@
     </row>
     <row r="297">
       <c r="A297" s="2" t="n">
-        <v>45777</v>
+        <v>25569.00000000789</v>
       </c>
       <c r="B297" t="inlineStr">
         <is>
@@ -22810,7 +22810,7 @@
     </row>
     <row r="298">
       <c r="A298" s="2" t="n">
-        <v>45624</v>
+        <v>25569.0000000039</v>
       </c>
       <c r="B298" t="inlineStr">
         <is>
@@ -22885,7 +22885,7 @@
     </row>
     <row r="299">
       <c r="A299" s="2" t="n">
-        <v>45689</v>
+        <v>25569.00000000317</v>
       </c>
       <c r="B299" t="inlineStr">
         <is>
@@ -22960,7 +22960,7 @@
     </row>
     <row r="300">
       <c r="A300" s="2" t="n">
-        <v>45528</v>
+        <v>25569.00000000098</v>
       </c>
       <c r="B300" t="inlineStr">
         <is>
@@ -23035,7 +23035,7 @@
     </row>
     <row r="301">
       <c r="A301" s="2" t="n">
-        <v>45744</v>
+        <v>25569.00000000175</v>
       </c>
       <c r="B301" t="inlineStr">
         <is>
@@ -23112,7 +23112,7 @@
     </row>
     <row r="302">
       <c r="A302" s="2" t="n">
-        <v>45567</v>
+        <v>25569.00000000242</v>
       </c>
       <c r="B302" t="inlineStr">
         <is>
@@ -23187,7 +23187,7 @@
     </row>
     <row r="303">
       <c r="A303" s="2" t="n">
-        <v>45560</v>
+        <v>25569.0000000019</v>
       </c>
       <c r="B303" t="inlineStr">
         <is>
@@ -23262,7 +23262,7 @@
     </row>
     <row r="304">
       <c r="A304" s="2" t="n">
-        <v>45563</v>
+        <v>25569.00000000087</v>
       </c>
       <c r="B304" t="inlineStr">
         <is>
@@ -23337,7 +23337,7 @@
     </row>
     <row r="305">
       <c r="A305" s="2" t="n">
-        <v>45497</v>
+        <v>25569.00000000205</v>
       </c>
       <c r="B305" t="inlineStr">
         <is>
@@ -23414,7 +23414,7 @@
     </row>
     <row r="306">
       <c r="A306" s="2" t="n">
-        <v>45772</v>
+        <v>25569.00000000042</v>
       </c>
       <c r="B306" t="inlineStr">
         <is>
@@ -23491,7 +23491,7 @@
     </row>
     <row r="307">
       <c r="A307" s="2" t="n">
-        <v>45700</v>
+        <v>25569.00000000184</v>
       </c>
       <c r="B307" t="inlineStr">
         <is>
@@ -23568,7 +23568,7 @@
     </row>
     <row r="308">
       <c r="A308" s="2" t="n">
-        <v>45723</v>
+        <v>25569.00000000627</v>
       </c>
       <c r="B308" t="inlineStr">
         <is>
@@ -23643,7 +23643,7 @@
     </row>
     <row r="309">
       <c r="A309" s="2" t="n">
-        <v>45566</v>
+        <v>25569.00000000406</v>
       </c>
       <c r="B309" t="inlineStr">
         <is>
@@ -23718,7 +23718,7 @@
     </row>
     <row r="310">
       <c r="A310" s="2" t="n">
-        <v>45521</v>
+        <v>25569.00000000432</v>
       </c>
       <c r="B310" t="inlineStr">
         <is>
@@ -23793,7 +23793,7 @@
     </row>
     <row r="311">
       <c r="A311" s="2" t="n">
-        <v>45762</v>
+        <v>25569.00000000115</v>
       </c>
       <c r="B311" t="inlineStr">
         <is>
@@ -23868,7 +23868,7 @@
     </row>
     <row r="312">
       <c r="A312" s="2" t="n">
-        <v>45832</v>
+        <v>25569.00000000428</v>
       </c>
       <c r="B312" t="inlineStr">
         <is>
@@ -23943,7 +23943,7 @@
     </row>
     <row r="313">
       <c r="A313" s="2" t="n">
-        <v>45784</v>
+        <v>25569.00000000127</v>
       </c>
       <c r="B313" t="inlineStr">
         <is>
@@ -24020,7 +24020,7 @@
     </row>
     <row r="314">
       <c r="A314" s="2" t="n">
-        <v>45753</v>
+        <v>25569.00000000446</v>
       </c>
       <c r="B314" t="inlineStr">
         <is>
@@ -24095,7 +24095,7 @@
     </row>
     <row r="315">
       <c r="A315" s="2" t="n">
-        <v>45518</v>
+        <v>25569.00000000767</v>
       </c>
       <c r="B315" t="inlineStr">
         <is>
@@ -24170,7 +24170,7 @@
     </row>
     <row r="316">
       <c r="A316" s="2" t="n">
-        <v>45605</v>
+        <v>25569.0000000227</v>
       </c>
       <c r="B316" t="inlineStr">
         <is>
@@ -24245,7 +24245,7 @@
     </row>
     <row r="317">
       <c r="A317" s="2" t="n">
-        <v>45689</v>
+        <v>25569.00000000207</v>
       </c>
       <c r="B317" t="inlineStr">
         <is>
@@ -24320,7 +24320,7 @@
     </row>
     <row r="318">
       <c r="A318" s="2" t="n">
-        <v>45574</v>
+        <v>25569.00000000077</v>
       </c>
       <c r="B318" t="inlineStr">
         <is>
@@ -24395,7 +24395,7 @@
     </row>
     <row r="319">
       <c r="A319" s="2" t="n">
-        <v>45854</v>
+        <v>25569.00000000313</v>
       </c>
       <c r="B319" t="inlineStr">
         <is>
@@ -24470,7 +24470,7 @@
     </row>
     <row r="320">
       <c r="A320" s="2" t="n">
-        <v>45592</v>
+        <v>25569.00000000465</v>
       </c>
       <c r="B320" t="inlineStr">
         <is>
@@ -24545,7 +24545,7 @@
     </row>
     <row r="321">
       <c r="A321" s="2" t="n">
-        <v>45674</v>
+        <v>25569.00000000075</v>
       </c>
       <c r="B321" t="inlineStr">
         <is>
@@ -24620,7 +24620,7 @@
     </row>
     <row r="322">
       <c r="A322" s="2" t="n">
-        <v>45522</v>
+        <v>25569.00000000314</v>
       </c>
       <c r="B322" t="inlineStr">
         <is>
@@ -24695,7 +24695,7 @@
     </row>
     <row r="323">
       <c r="A323" s="2" t="n">
-        <v>45756</v>
+        <v>25569.00000000413</v>
       </c>
       <c r="B323" t="inlineStr">
         <is>
@@ -24770,7 +24770,7 @@
     </row>
     <row r="324">
       <c r="A324" s="2" t="n">
-        <v>45611</v>
+        <v>25569.00000000677</v>
       </c>
       <c r="B324" t="inlineStr">
         <is>
@@ -24845,7 +24845,7 @@
     </row>
     <row r="325">
       <c r="A325" s="2" t="n">
-        <v>45508</v>
+        <v>25569.00000000211</v>
       </c>
       <c r="B325" t="inlineStr">
         <is>
@@ -24920,7 +24920,7 @@
     </row>
     <row r="326">
       <c r="A326" s="2" t="n">
-        <v>45595</v>
+        <v>25569.00000000186</v>
       </c>
       <c r="B326" t="inlineStr">
         <is>
@@ -24995,7 +24995,7 @@
     </row>
     <row r="327">
       <c r="A327" s="2" t="n">
-        <v>45525</v>
+        <v>25569.00000000545</v>
       </c>
       <c r="B327" t="inlineStr">
         <is>
@@ -25070,7 +25070,7 @@
     </row>
     <row r="328">
       <c r="A328" s="2" t="n">
-        <v>45850</v>
+        <v>25569.00000000214</v>
       </c>
       <c r="B328" t="inlineStr">
         <is>
@@ -25145,7 +25145,7 @@
     </row>
     <row r="329">
       <c r="A329" s="2" t="n">
-        <v>45523</v>
+        <v>25569.00000002155</v>
       </c>
       <c r="B329" t="inlineStr">
         <is>
@@ -25220,7 +25220,7 @@
     </row>
     <row r="330">
       <c r="A330" s="2" t="n">
-        <v>45734</v>
+        <v>25569.00000000933</v>
       </c>
       <c r="B330" t="inlineStr">
         <is>
@@ -25295,7 +25295,7 @@
     </row>
     <row r="331">
       <c r="A331" s="2" t="n">
-        <v>45663</v>
+        <v>25569.00000000688</v>
       </c>
       <c r="B331" t="inlineStr">
         <is>
@@ -25370,7 +25370,7 @@
     </row>
     <row r="332">
       <c r="A332" s="2" t="n">
-        <v>45770</v>
+        <v>25569.00000000124</v>
       </c>
       <c r="B332" t="inlineStr">
         <is>
@@ -25445,7 +25445,7 @@
     </row>
     <row r="333">
       <c r="A333" s="2" t="n">
-        <v>45517</v>
+        <v>25569.00000000108</v>
       </c>
       <c r="B333" t="inlineStr">
         <is>
@@ -25520,7 +25520,7 @@
     </row>
     <row r="334">
       <c r="A334" s="2" t="n">
-        <v>45709</v>
+        <v>25569.0000000033</v>
       </c>
       <c r="B334" t="inlineStr">
         <is>
@@ -25595,7 +25595,7 @@
     </row>
     <row r="335">
       <c r="A335" s="2" t="n">
-        <v>45737</v>
+        <v>25569.00000000494</v>
       </c>
       <c r="B335" t="inlineStr">
         <is>
@@ -25670,7 +25670,7 @@
     </row>
     <row r="336">
       <c r="A336" s="2" t="n">
-        <v>45576</v>
+        <v>25569.00000000158</v>
       </c>
       <c r="B336" t="inlineStr">
         <is>
@@ -25745,7 +25745,7 @@
     </row>
     <row r="337">
       <c r="A337" s="2" t="n">
-        <v>45550</v>
+        <v>25569.00000000912</v>
       </c>
       <c r="B337" t="inlineStr">
         <is>
@@ -25822,7 +25822,7 @@
     </row>
     <row r="338">
       <c r="A338" s="2" t="n">
-        <v>45856</v>
+        <v>25569.00000001092</v>
       </c>
       <c r="B338" t="inlineStr">
         <is>
@@ -25897,7 +25897,7 @@
     </row>
     <row r="339">
       <c r="A339" s="2" t="n">
-        <v>45701</v>
+        <v>25569.00000000353</v>
       </c>
       <c r="B339" t="inlineStr">
         <is>
@@ -25972,7 +25972,7 @@
     </row>
     <row r="340">
       <c r="A340" s="2" t="n">
-        <v>45691</v>
+        <v>25569.00000000192</v>
       </c>
       <c r="B340" t="inlineStr">
         <is>
@@ -26047,7 +26047,7 @@
     </row>
     <row r="341">
       <c r="A341" s="2" t="n">
-        <v>45570</v>
+        <v>25569.00000000095</v>
       </c>
       <c r="B341" t="inlineStr">
         <is>
@@ -26122,7 +26122,7 @@
     </row>
     <row r="342">
       <c r="A342" s="2" t="n">
-        <v>45755</v>
+        <v>25569.00000000737</v>
       </c>
       <c r="B342" t="inlineStr">
         <is>
@@ -26197,7 +26197,7 @@
     </row>
     <row r="343">
       <c r="A343" s="2" t="n">
-        <v>45514</v>
+        <v>25569.00000000232</v>
       </c>
       <c r="B343" t="inlineStr">
         <is>
@@ -26272,7 +26272,7 @@
     </row>
     <row r="344">
       <c r="A344" s="2" t="n">
-        <v>45597</v>
+        <v>25569.00000000403</v>
       </c>
       <c r="B344" t="inlineStr">
         <is>
@@ -26347,7 +26347,7 @@
     </row>
     <row r="345">
       <c r="A345" s="2" t="n">
-        <v>45554</v>
+        <v>25569.0000000017</v>
       </c>
       <c r="B345" t="inlineStr">
         <is>
@@ -26422,7 +26422,7 @@
     </row>
     <row r="346">
       <c r="A346" s="2" t="n">
-        <v>45772</v>
+        <v>25569.00000000218</v>
       </c>
       <c r="B346" t="inlineStr">
         <is>
@@ -26499,7 +26499,7 @@
     </row>
     <row r="347">
       <c r="A347" s="2" t="n">
-        <v>45780</v>
+        <v>25569.00000000158</v>
       </c>
       <c r="B347" t="inlineStr">
         <is>
@@ -26576,7 +26576,7 @@
     </row>
     <row r="348">
       <c r="A348" s="2" t="n">
-        <v>45753</v>
+        <v>25569.00000000146</v>
       </c>
       <c r="B348" t="inlineStr">
         <is>
@@ -26651,7 +26651,7 @@
     </row>
     <row r="349">
       <c r="A349" s="2" t="n">
-        <v>45858</v>
+        <v>25569.00000000189</v>
       </c>
       <c r="B349" t="inlineStr">
         <is>
@@ -26728,7 +26728,7 @@
     </row>
     <row r="350">
       <c r="A350" s="2" t="n">
-        <v>45817</v>
+        <v>25569.00000000494</v>
       </c>
       <c r="B350" t="inlineStr">
         <is>
@@ -26805,7 +26805,7 @@
     </row>
     <row r="351">
       <c r="A351" s="2" t="n">
-        <v>45817</v>
+        <v>25569.00000000979</v>
       </c>
       <c r="B351" t="inlineStr">
         <is>
@@ -26880,7 +26880,7 @@
     </row>
     <row r="352">
       <c r="A352" s="2" t="n">
-        <v>45767</v>
+        <v>25569.00000000159</v>
       </c>
       <c r="B352" t="inlineStr">
         <is>
@@ -26955,7 +26955,7 @@
     </row>
     <row r="353">
       <c r="A353" s="2" t="n">
-        <v>45514</v>
+        <v>25569.00000000051</v>
       </c>
       <c r="B353" t="inlineStr">
         <is>
@@ -27030,7 +27030,7 @@
     </row>
     <row r="354">
       <c r="A354" s="2" t="n">
-        <v>45766</v>
+        <v>25569.00000000625</v>
       </c>
       <c r="B354" t="inlineStr">
         <is>
@@ -27105,7 +27105,7 @@
     </row>
     <row r="355">
       <c r="A355" s="2" t="n">
-        <v>45756</v>
+        <v>25569.00000001079</v>
       </c>
       <c r="B355" t="inlineStr">
         <is>
@@ -27180,7 +27180,7 @@
     </row>
     <row r="356">
       <c r="A356" s="2" t="n">
-        <v>45678</v>
+        <v>25569.00000000131</v>
       </c>
       <c r="B356" t="inlineStr">
         <is>
@@ -27255,7 +27255,7 @@
     </row>
     <row r="357">
       <c r="A357" s="2" t="n">
-        <v>45810</v>
+        <v>25569.00000000136</v>
       </c>
       <c r="B357" t="inlineStr">
         <is>
@@ -27330,7 +27330,7 @@
     </row>
     <row r="358">
       <c r="A358" s="2" t="n">
-        <v>45813</v>
+        <v>25569.00000000561</v>
       </c>
       <c r="B358" t="inlineStr">
         <is>
@@ -27405,7 +27405,7 @@
     </row>
     <row r="359">
       <c r="A359" s="2" t="n">
-        <v>45688</v>
+        <v>25569.00000000471</v>
       </c>
       <c r="B359" t="inlineStr">
         <is>
@@ -27480,7 +27480,7 @@
     </row>
     <row r="360">
       <c r="A360" s="2" t="n">
-        <v>45631</v>
+        <v>25569.00000000576</v>
       </c>
       <c r="B360" t="inlineStr">
         <is>
@@ -27555,7 +27555,7 @@
     </row>
     <row r="361">
       <c r="A361" s="2" t="n">
-        <v>45711</v>
+        <v>25569.00000000592</v>
       </c>
       <c r="B361" t="inlineStr">
         <is>
@@ -27630,7 +27630,7 @@
     </row>
     <row r="362">
       <c r="A362" s="2" t="n">
-        <v>45824</v>
+        <v>25569.00000000152</v>
       </c>
       <c r="B362" t="inlineStr">
         <is>
@@ -27705,7 +27705,7 @@
     </row>
     <row r="363">
       <c r="A363" s="2" t="n">
-        <v>45828</v>
+        <v>25569.00000000473</v>
       </c>
       <c r="B363" t="inlineStr">
         <is>
@@ -27780,7 +27780,7 @@
     </row>
     <row r="364">
       <c r="A364" s="2" t="n">
-        <v>45730</v>
+        <v>25569.000000001</v>
       </c>
       <c r="B364" t="inlineStr">
         <is>
@@ -27857,7 +27857,7 @@
     </row>
     <row r="365">
       <c r="A365" s="2" t="n">
-        <v>45547</v>
+        <v>25569.00000000215</v>
       </c>
       <c r="B365" t="inlineStr">
         <is>
@@ -27932,7 +27932,7 @@
     </row>
     <row r="366">
       <c r="A366" s="2" t="n">
-        <v>45530</v>
+        <v>25569.00000000104</v>
       </c>
       <c r="B366" t="inlineStr">
         <is>
@@ -28007,7 +28007,7 @@
     </row>
     <row r="367">
       <c r="A367" s="2" t="n">
-        <v>45573</v>
+        <v>25569.0000000057</v>
       </c>
       <c r="B367" t="inlineStr">
         <is>
@@ -28082,7 +28082,7 @@
     </row>
     <row r="368">
       <c r="A368" s="2" t="n">
-        <v>45731</v>
+        <v>25569.0000000014</v>
       </c>
       <c r="B368" t="inlineStr">
         <is>
@@ -28159,7 +28159,7 @@
     </row>
     <row r="369">
       <c r="A369" s="2" t="n">
-        <v>45682</v>
+        <v>25569.00000000413</v>
       </c>
       <c r="B369" t="inlineStr">
         <is>
@@ -28234,7 +28234,7 @@
     </row>
     <row r="370">
       <c r="A370" s="2" t="n">
-        <v>45848</v>
+        <v>25569.00000000249</v>
       </c>
       <c r="B370" t="inlineStr">
         <is>
@@ -28309,7 +28309,7 @@
     </row>
     <row r="371">
       <c r="A371" s="2" t="n">
-        <v>45854</v>
+        <v>25569.00000000089</v>
       </c>
       <c r="B371" t="inlineStr">
         <is>
@@ -28384,7 +28384,7 @@
     </row>
     <row r="372">
       <c r="A372" s="2" t="n">
-        <v>45506</v>
+        <v>25569.00000000544</v>
       </c>
       <c r="B372" t="inlineStr">
         <is>
@@ -28459,7 +28459,7 @@
     </row>
     <row r="373">
       <c r="A373" s="2" t="n">
-        <v>45510</v>
+        <v>25569.00000000174</v>
       </c>
       <c r="B373" t="inlineStr">
         <is>
@@ -28534,7 +28534,7 @@
     </row>
     <row r="374">
       <c r="A374" s="2" t="n">
-        <v>45680</v>
+        <v>25569.00000000677</v>
       </c>
       <c r="B374" t="inlineStr">
         <is>
@@ -28609,7 +28609,7 @@
     </row>
     <row r="375">
       <c r="A375" s="2" t="n">
-        <v>45530</v>
+        <v>25569.00000000709</v>
       </c>
       <c r="B375" t="inlineStr">
         <is>
@@ -28684,7 +28684,7 @@
     </row>
     <row r="376">
       <c r="A376" s="2" t="n">
-        <v>45731</v>
+        <v>25569.00000001145</v>
       </c>
       <c r="B376" t="inlineStr">
         <is>
@@ -28759,7 +28759,7 @@
     </row>
     <row r="377">
       <c r="A377" s="2" t="n">
-        <v>45778</v>
+        <v>25569.00000000374</v>
       </c>
       <c r="B377" t="inlineStr">
         <is>
@@ -28834,7 +28834,7 @@
     </row>
     <row r="378">
       <c r="A378" s="2" t="n">
-        <v>45798</v>
+        <v>25569.00000000459</v>
       </c>
       <c r="B378" t="inlineStr">
         <is>
@@ -28909,7 +28909,7 @@
     </row>
     <row r="379">
       <c r="A379" s="2" t="n">
-        <v>45657</v>
+        <v>25569.00000001053</v>
       </c>
       <c r="B379" t="inlineStr">
         <is>
@@ -28984,7 +28984,7 @@
     </row>
     <row r="380">
       <c r="A380" s="2" t="n">
-        <v>45735</v>
+        <v>25569.00000000264</v>
       </c>
       <c r="B380" t="inlineStr">
         <is>
@@ -29059,7 +29059,7 @@
     </row>
     <row r="381">
       <c r="A381" s="2" t="n">
-        <v>45612</v>
+        <v>25569.00000000541</v>
       </c>
       <c r="B381" t="inlineStr">
         <is>
@@ -29134,7 +29134,7 @@
     </row>
     <row r="382">
       <c r="A382" s="2" t="n">
-        <v>45826</v>
+        <v>25569.00000000098</v>
       </c>
       <c r="B382" t="inlineStr">
         <is>
@@ -29209,7 +29209,7 @@
     </row>
     <row r="383">
       <c r="A383" s="2" t="n">
-        <v>45660</v>
+        <v>25569.00000000134</v>
       </c>
       <c r="B383" t="inlineStr">
         <is>
@@ -29286,7 +29286,7 @@
     </row>
     <row r="384">
       <c r="A384" s="2" t="n">
-        <v>45706</v>
+        <v>25569.00000000436</v>
       </c>
       <c r="B384" t="inlineStr">
         <is>
@@ -29361,7 +29361,7 @@
     </row>
     <row r="385">
       <c r="A385" s="2" t="n">
-        <v>45782</v>
+        <v>25569.00000000411</v>
       </c>
       <c r="B385" t="inlineStr">
         <is>
@@ -29436,7 +29436,7 @@
     </row>
     <row r="386">
       <c r="A386" s="2" t="n">
-        <v>45794</v>
+        <v>25569.00000001001</v>
       </c>
       <c r="B386" t="inlineStr">
         <is>
@@ -29511,7 +29511,7 @@
     </row>
     <row r="387">
       <c r="A387" s="2" t="n">
-        <v>45849</v>
+        <v>25569.00000001045</v>
       </c>
       <c r="B387" t="inlineStr">
         <is>
@@ -29586,7 +29586,7 @@
     </row>
     <row r="388">
       <c r="A388" s="2" t="n">
-        <v>45622</v>
+        <v>25569.00000000023</v>
       </c>
       <c r="B388" t="inlineStr">
         <is>
@@ -29661,7 +29661,7 @@
     </row>
     <row r="389">
       <c r="A389" s="2" t="n">
-        <v>45587</v>
+        <v>25569.00000000414</v>
       </c>
       <c r="B389" t="inlineStr">
         <is>
@@ -29738,7 +29738,7 @@
     </row>
     <row r="390">
       <c r="A390" s="2" t="n">
-        <v>45713</v>
+        <v>25569.00000000474</v>
       </c>
       <c r="B390" t="inlineStr">
         <is>
@@ -29815,7 +29815,7 @@
     </row>
     <row r="391">
       <c r="A391" s="2" t="n">
-        <v>45603</v>
+        <v>25569.00000000338</v>
       </c>
       <c r="B391" t="inlineStr">
         <is>
@@ -29890,7 +29890,7 @@
     </row>
     <row r="392">
       <c r="A392" s="2" t="n">
-        <v>45847</v>
+        <v>25569.00000000206</v>
       </c>
       <c r="B392" t="inlineStr">
         <is>
@@ -29967,7 +29967,7 @@
     </row>
     <row r="393">
       <c r="A393" s="2" t="n">
-        <v>45809</v>
+        <v>25569.00000000125</v>
       </c>
       <c r="B393" t="inlineStr">
         <is>
@@ -30042,7 +30042,7 @@
     </row>
     <row r="394">
       <c r="A394" s="2" t="n">
-        <v>45817</v>
+        <v>25569.0000000052</v>
       </c>
       <c r="B394" t="inlineStr">
         <is>
@@ -30117,7 +30117,7 @@
     </row>
     <row r="395">
       <c r="A395" s="2" t="n">
-        <v>45535</v>
+        <v>25569.00000000197</v>
       </c>
       <c r="B395" t="inlineStr">
         <is>
@@ -30192,7 +30192,7 @@
     </row>
     <row r="396">
       <c r="A396" s="2" t="n">
-        <v>45811</v>
+        <v>25569.00000000585</v>
       </c>
       <c r="B396" t="inlineStr">
         <is>
@@ -30267,7 +30267,7 @@
     </row>
     <row r="397">
       <c r="A397" s="2" t="n">
-        <v>45568</v>
+        <v>25569.00000000183</v>
       </c>
       <c r="B397" t="inlineStr">
         <is>
@@ -30342,7 +30342,7 @@
     </row>
     <row r="398">
       <c r="A398" s="2" t="n">
-        <v>45559</v>
+        <v>25569.00000000162</v>
       </c>
       <c r="B398" t="inlineStr">
         <is>
@@ -30417,7 +30417,7 @@
     </row>
     <row r="399">
       <c r="A399" s="2" t="n">
-        <v>45523</v>
+        <v>25569.00000000097</v>
       </c>
       <c r="B399" t="inlineStr">
         <is>
@@ -30492,7 +30492,7 @@
     </row>
     <row r="400">
       <c r="A400" s="2" t="n">
-        <v>45766</v>
+        <v>25569.00000000228</v>
       </c>
       <c r="B400" t="inlineStr">
         <is>
@@ -30567,7 +30567,7 @@
     </row>
     <row r="401">
       <c r="A401" s="2" t="n">
-        <v>45722</v>
+        <v>25569.00000000567</v>
       </c>
       <c r="B401" t="inlineStr">
         <is>
@@ -30642,7 +30642,7 @@
     </row>
     <row r="402">
       <c r="A402" s="2" t="n">
-        <v>45646</v>
+        <v>25569.00000000167</v>
       </c>
       <c r="B402" t="inlineStr">
         <is>
@@ -30717,7 +30717,7 @@
     </row>
     <row r="403">
       <c r="A403" s="2" t="n">
-        <v>45798</v>
+        <v>25569.00000000435</v>
       </c>
       <c r="B403" t="inlineStr">
         <is>
@@ -30792,7 +30792,7 @@
     </row>
     <row r="404">
       <c r="A404" s="2" t="n">
-        <v>45858</v>
+        <v>25569.00000000298</v>
       </c>
       <c r="B404" t="inlineStr">
         <is>
@@ -30869,7 +30869,7 @@
     </row>
     <row r="405">
       <c r="A405" s="2" t="n">
-        <v>45562</v>
+        <v>25569.00000000215</v>
       </c>
       <c r="B405" t="inlineStr">
         <is>
@@ -30944,7 +30944,7 @@
     </row>
     <row r="406">
       <c r="A406" s="2" t="n">
-        <v>45727</v>
+        <v>25569.00000000081</v>
       </c>
       <c r="B406" t="inlineStr">
         <is>
@@ -31019,7 +31019,7 @@
     </row>
     <row r="407">
       <c r="A407" s="2" t="n">
-        <v>45505</v>
+        <v>25569.00000000186</v>
       </c>
       <c r="B407" t="inlineStr">
         <is>
@@ -31094,7 +31094,7 @@
     </row>
     <row r="408">
       <c r="A408" s="2" t="n">
-        <v>45686</v>
+        <v>25569.00000000158</v>
       </c>
       <c r="B408" t="inlineStr">
         <is>
@@ -31169,7 +31169,7 @@
     </row>
     <row r="409">
       <c r="A409" s="2" t="n">
-        <v>45505</v>
+        <v>25569.0000000105</v>
       </c>
       <c r="B409" t="inlineStr">
         <is>
@@ -31244,7 +31244,7 @@
     </row>
     <row r="410">
       <c r="A410" s="2" t="n">
-        <v>45549</v>
+        <v>25569.00000000366</v>
       </c>
       <c r="B410" t="inlineStr">
         <is>
@@ -31319,7 +31319,7 @@
     </row>
     <row r="411">
       <c r="A411" s="2" t="n">
-        <v>45597</v>
+        <v>25569.00000000249</v>
       </c>
       <c r="B411" t="inlineStr">
         <is>
@@ -31394,7 +31394,7 @@
     </row>
     <row r="412">
       <c r="A412" s="2" t="n">
-        <v>45769</v>
+        <v>25569.00000000107</v>
       </c>
       <c r="B412" t="inlineStr">
         <is>
@@ -31469,7 +31469,7 @@
     </row>
     <row r="413">
       <c r="A413" s="2" t="n">
-        <v>45724</v>
+        <v>25569.00000000401</v>
       </c>
       <c r="B413" t="inlineStr">
         <is>
@@ -31544,7 +31544,7 @@
     </row>
     <row r="414">
       <c r="A414" s="2" t="n">
-        <v>45819</v>
+        <v>25569.00000000802</v>
       </c>
       <c r="B414" t="inlineStr">
         <is>
@@ -31619,7 +31619,7 @@
     </row>
     <row r="415">
       <c r="A415" s="2" t="n">
-        <v>45606</v>
+        <v>25569.00000000575</v>
       </c>
       <c r="B415" t="inlineStr">
         <is>
@@ -31694,7 +31694,7 @@
     </row>
     <row r="416">
       <c r="A416" s="2" t="n">
-        <v>45589</v>
+        <v>25569.00000000489</v>
       </c>
       <c r="B416" t="inlineStr">
         <is>
@@ -31769,7 +31769,7 @@
     </row>
     <row r="417">
       <c r="A417" s="2" t="n">
-        <v>45665</v>
+        <v>25569.00000000515</v>
       </c>
       <c r="B417" t="inlineStr">
         <is>
@@ -31844,7 +31844,7 @@
     </row>
     <row r="418">
       <c r="A418" s="2" t="n">
-        <v>45516</v>
+        <v>25569.00000000781</v>
       </c>
       <c r="B418" t="inlineStr">
         <is>
@@ -31921,7 +31921,7 @@
     </row>
     <row r="419">
       <c r="A419" s="2" t="n">
-        <v>45723</v>
+        <v>25569.00000000541</v>
       </c>
       <c r="B419" t="inlineStr">
         <is>
@@ -31996,7 +31996,7 @@
     </row>
     <row r="420">
       <c r="A420" s="2" t="n">
-        <v>45855</v>
+        <v>25569.00000000107</v>
       </c>
       <c r="B420" t="inlineStr">
         <is>
@@ -32071,7 +32071,7 @@
     </row>
     <row r="421">
       <c r="A421" s="2" t="n">
-        <v>45852</v>
+        <v>25569.00000001691</v>
       </c>
       <c r="B421" t="inlineStr">
         <is>
@@ -32146,7 +32146,7 @@
     </row>
     <row r="422">
       <c r="A422" s="2" t="n">
-        <v>45643</v>
+        <v>25569.00000001054</v>
       </c>
       <c r="B422" t="inlineStr">
         <is>
@@ -32221,7 +32221,7 @@
     </row>
     <row r="423">
       <c r="A423" s="2" t="n">
-        <v>45625</v>
+        <v>25569.00000000032</v>
       </c>
       <c r="B423" t="inlineStr">
         <is>
@@ -32296,7 +32296,7 @@
     </row>
     <row r="424">
       <c r="A424" s="2" t="n">
-        <v>45818</v>
+        <v>25569.00000000202</v>
       </c>
       <c r="B424" t="inlineStr">
         <is>
@@ -32371,7 +32371,7 @@
     </row>
     <row r="425">
       <c r="A425" s="2" t="n">
-        <v>45708</v>
+        <v>25569.00000002274</v>
       </c>
       <c r="B425" t="inlineStr">
         <is>
@@ -32446,7 +32446,7 @@
     </row>
     <row r="426">
       <c r="A426" s="2" t="n">
-        <v>45849</v>
+        <v>25569.00000000196</v>
       </c>
       <c r="B426" t="inlineStr">
         <is>
@@ -32521,7 +32521,7 @@
     </row>
     <row r="427">
       <c r="A427" s="2" t="n">
-        <v>45758</v>
+        <v>25569.00000000119</v>
       </c>
       <c r="B427" t="inlineStr">
         <is>
@@ -32596,7 +32596,7 @@
     </row>
     <row r="428">
       <c r="A428" s="2" t="n">
-        <v>45835</v>
+        <v>25569.00000000322</v>
       </c>
       <c r="B428" t="inlineStr">
         <is>
@@ -32671,7 +32671,7 @@
     </row>
     <row r="429">
       <c r="A429" s="2" t="n">
-        <v>45611</v>
+        <v>25569.00000000107</v>
       </c>
       <c r="B429" t="inlineStr">
         <is>
@@ -32748,7 +32748,7 @@
     </row>
     <row r="430">
       <c r="A430" s="2" t="n">
-        <v>45743</v>
+        <v>25569.00000000126</v>
       </c>
       <c r="B430" t="inlineStr">
         <is>
@@ -32823,7 +32823,7 @@
     </row>
     <row r="431">
       <c r="A431" s="2" t="n">
-        <v>45567</v>
+        <v>25569.00000000083</v>
       </c>
       <c r="B431" t="inlineStr">
         <is>
@@ -32898,7 +32898,7 @@
     </row>
     <row r="432">
       <c r="A432" s="2" t="n">
-        <v>45743</v>
+        <v>25569.00000000183</v>
       </c>
       <c r="B432" t="inlineStr">
         <is>
@@ -32973,7 +32973,7 @@
     </row>
     <row r="433">
       <c r="A433" s="2" t="n">
-        <v>45686</v>
+        <v>25569.00000000083</v>
       </c>
       <c r="B433" t="inlineStr">
         <is>
@@ -33048,7 +33048,7 @@
     </row>
     <row r="434">
       <c r="A434" s="2" t="n">
-        <v>45662</v>
+        <v>25569.00000000095</v>
       </c>
       <c r="B434" t="inlineStr">
         <is>
@@ -33123,7 +33123,7 @@
     </row>
     <row r="435">
       <c r="A435" s="2" t="n">
-        <v>45553</v>
+        <v>25569.00000000112</v>
       </c>
       <c r="B435" t="inlineStr">
         <is>
@@ -33198,7 +33198,7 @@
     </row>
     <row r="436">
       <c r="A436" s="2" t="n">
-        <v>45585</v>
+        <v>25569.00000000219</v>
       </c>
       <c r="B436" t="inlineStr">
         <is>
@@ -33275,7 +33275,7 @@
     </row>
     <row r="437">
       <c r="A437" s="2" t="n">
-        <v>45570</v>
+        <v>25569.00000000134</v>
       </c>
       <c r="B437" t="inlineStr">
         <is>
@@ -33350,7 +33350,7 @@
     </row>
     <row r="438">
       <c r="A438" s="2" t="n">
-        <v>45848</v>
+        <v>25569.00000000207</v>
       </c>
       <c r="B438" t="inlineStr">
         <is>
@@ -33425,7 +33425,7 @@
     </row>
     <row r="439">
       <c r="A439" s="2" t="n">
-        <v>45521</v>
+        <v>25569.00000000229</v>
       </c>
       <c r="B439" t="inlineStr">
         <is>
@@ -33502,7 +33502,7 @@
     </row>
     <row r="440">
       <c r="A440" s="2" t="n">
-        <v>45621</v>
+        <v>25569.00000000342</v>
       </c>
       <c r="B440" t="inlineStr">
         <is>
@@ -33579,7 +33579,7 @@
     </row>
     <row r="441">
       <c r="A441" s="2" t="n">
-        <v>45820</v>
+        <v>25569.00000000534</v>
       </c>
       <c r="B441" t="inlineStr">
         <is>
@@ -33654,7 +33654,7 @@
     </row>
     <row r="442">
       <c r="A442" s="2" t="n">
-        <v>45564</v>
+        <v>25569.00000000038</v>
       </c>
       <c r="B442" t="inlineStr">
         <is>
@@ -33729,7 +33729,7 @@
     </row>
     <row r="443">
       <c r="A443" s="2" t="n">
-        <v>45723</v>
+        <v>25569.00000000412</v>
       </c>
       <c r="B443" t="inlineStr">
         <is>
@@ -33804,7 +33804,7 @@
     </row>
     <row r="444">
       <c r="A444" s="2" t="n">
-        <v>45699</v>
+        <v>25569.0000000107</v>
       </c>
       <c r="B444" t="inlineStr">
         <is>
@@ -33881,7 +33881,7 @@
     </row>
     <row r="445">
       <c r="A445" s="2" t="n">
-        <v>45656</v>
+        <v>25569.00000000691</v>
       </c>
       <c r="B445" t="inlineStr">
         <is>
@@ -33956,7 +33956,7 @@
     </row>
     <row r="446">
       <c r="A446" s="2" t="n">
-        <v>45836</v>
+        <v>25569.00000000844</v>
       </c>
       <c r="B446" t="inlineStr">
         <is>
@@ -34031,7 +34031,7 @@
     </row>
     <row r="447">
       <c r="A447" s="2" t="n">
-        <v>45793</v>
+        <v>25569.00000000167</v>
       </c>
       <c r="B447" t="inlineStr">
         <is>
@@ -34106,7 +34106,7 @@
     </row>
     <row r="448">
       <c r="A448" s="2" t="n">
-        <v>45662</v>
+        <v>25569.00000000066</v>
       </c>
       <c r="B448" t="inlineStr">
         <is>
@@ -34181,7 +34181,7 @@
     </row>
     <row r="449">
       <c r="A449" s="2" t="n">
-        <v>45812</v>
+        <v>25569.00000000186</v>
       </c>
       <c r="B449" t="inlineStr">
         <is>
@@ -34256,7 +34256,7 @@
     </row>
     <row r="450">
       <c r="A450" s="2" t="n">
-        <v>45556</v>
+        <v>25569.00000000283</v>
       </c>
       <c r="B450" t="inlineStr">
         <is>
@@ -34331,7 +34331,7 @@
     </row>
     <row r="451">
       <c r="A451" s="2" t="n">
-        <v>45738</v>
+        <v>25569.00000000125</v>
       </c>
       <c r="B451" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
full ai and ml
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -2433,7 +2433,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (ML)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (ML)</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -5441,7 +5441,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -18391,7 +18391,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (ML)</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -19743,7 +19743,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -23590,7 +23590,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (ML)</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -24717,7 +24717,7 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G323" t="inlineStr">
@@ -25844,7 +25844,7 @@
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (ML)</t>
         </is>
       </c>
       <c r="G338" t="inlineStr">
@@ -26598,7 +26598,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (ML)</t>
         </is>
       </c>
       <c r="G348" t="inlineStr">
@@ -28481,7 +28481,7 @@
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (ML)</t>
         </is>
       </c>
       <c r="G373" t="inlineStr">

</xml_diff>

<commit_message>
reveue anlisis ollam a
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -548,7 +548,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (ML)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -4539,7 +4539,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -9815,7 +9815,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
@@ -11396,7 +11396,7 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
@@ -19743,7 +19743,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (ML)</t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -23590,7 +23590,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -24717,7 +24717,7 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Financing Activities (ML)</t>
         </is>
       </c>
       <c r="G323" t="inlineStr">
@@ -26598,7 +26598,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (ML)</t>
         </is>
       </c>
       <c r="G348" t="inlineStr">

</xml_diff>

<commit_message>
changes mde with no errors
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -548,7 +548,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -625,7 +625,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1302,7 +1302,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1377,7 +1377,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2208,7 +2208,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2283,7 +2283,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2358,7 +2358,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2733,7 +2733,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2883,7 +2883,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -3183,7 +3183,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -3333,7 +3333,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -3408,7 +3408,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -3485,7 +3485,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -3939,7 +3939,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -4014,7 +4014,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -4239,7 +4239,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -4464,7 +4464,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -4539,7 +4539,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -4614,7 +4614,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -4689,7 +4689,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -4764,7 +4764,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -4839,7 +4839,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -4916,7 +4916,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -5066,7 +5066,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -5141,7 +5141,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -5291,7 +5291,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -5366,7 +5366,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -5441,7 +5441,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -5591,7 +5591,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -5666,7 +5666,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -5741,7 +5741,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -5891,7 +5891,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -5966,7 +5966,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -6041,7 +6041,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -6118,7 +6118,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -6193,7 +6193,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -6268,7 +6268,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -6343,7 +6343,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -6418,7 +6418,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -6495,7 +6495,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -6572,7 +6572,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -6649,7 +6649,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -6724,7 +6724,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -6799,7 +6799,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -6874,7 +6874,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -6951,7 +6951,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -7026,7 +7026,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -7101,7 +7101,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -7176,7 +7176,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -7251,7 +7251,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -7326,7 +7326,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -7476,7 +7476,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -7551,7 +7551,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -7626,7 +7626,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -7701,7 +7701,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -7776,7 +7776,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -7851,7 +7851,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -8001,7 +8001,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -8078,7 +8078,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -8153,7 +8153,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -8228,7 +8228,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -8303,7 +8303,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -8380,7 +8380,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -8455,7 +8455,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -8530,7 +8530,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -8605,7 +8605,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -8682,7 +8682,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -8757,7 +8757,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -8832,7 +8832,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -8907,7 +8907,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -8982,7 +8982,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -9057,7 +9057,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -9132,7 +9132,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -9207,7 +9207,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -9282,7 +9282,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -9359,7 +9359,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -9436,7 +9436,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -9511,7 +9511,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -9586,7 +9586,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -9661,7 +9661,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -9738,7 +9738,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -9815,7 +9815,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
@@ -9890,7 +9890,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -9965,7 +9965,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -10040,7 +10040,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
@@ -10115,7 +10115,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
@@ -10190,7 +10190,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -10267,7 +10267,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
@@ -10342,7 +10342,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -10417,7 +10417,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -10492,7 +10492,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -10569,7 +10569,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -10644,7 +10644,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -10719,7 +10719,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
@@ -10794,7 +10794,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -10869,7 +10869,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -10944,7 +10944,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
@@ -11021,7 +11021,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
@@ -11096,7 +11096,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -11171,7 +11171,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
@@ -11246,7 +11246,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -11321,7 +11321,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -11396,7 +11396,7 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
@@ -11471,7 +11471,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -11546,7 +11546,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
@@ -11621,7 +11621,7 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
@@ -11696,7 +11696,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -11771,7 +11771,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
@@ -11846,7 +11846,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -11921,7 +11921,7 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
@@ -11996,7 +11996,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
@@ -12071,7 +12071,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
@@ -12148,7 +12148,7 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
@@ -12225,7 +12225,7 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
@@ -12300,7 +12300,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -12375,7 +12375,7 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
@@ -12450,7 +12450,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
@@ -12525,7 +12525,7 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
@@ -12600,7 +12600,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
@@ -12675,7 +12675,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
@@ -12750,7 +12750,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
@@ -12825,7 +12825,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
@@ -12900,7 +12900,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
@@ -12975,7 +12975,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
@@ -13050,7 +13050,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
@@ -13125,7 +13125,7 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G169" t="inlineStr">
@@ -13200,7 +13200,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
@@ -13275,7 +13275,7 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
@@ -13350,7 +13350,7 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G172" t="inlineStr">
@@ -13425,7 +13425,7 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
@@ -13502,7 +13502,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
@@ -13579,7 +13579,7 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
@@ -13654,7 +13654,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
@@ -13729,7 +13729,7 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G177" t="inlineStr">
@@ -13804,7 +13804,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
@@ -13879,7 +13879,7 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
@@ -13954,7 +13954,7 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
@@ -14029,7 +14029,7 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
@@ -14104,7 +14104,7 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G182" t="inlineStr">
@@ -14179,7 +14179,7 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
@@ -14254,7 +14254,7 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
@@ -14329,7 +14329,7 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
@@ -14404,7 +14404,7 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G186" t="inlineStr">
@@ -14479,7 +14479,7 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
@@ -14554,7 +14554,7 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
@@ -14629,7 +14629,7 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
@@ -14704,7 +14704,7 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
@@ -14779,7 +14779,7 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G191" t="inlineStr">
@@ -14854,7 +14854,7 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G192" t="inlineStr">
@@ -14929,7 +14929,7 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
@@ -15004,7 +15004,7 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
@@ -15079,7 +15079,7 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
@@ -15154,7 +15154,7 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
@@ -15229,7 +15229,7 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
@@ -15306,7 +15306,7 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G198" t="inlineStr">
@@ -15381,7 +15381,7 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
@@ -15456,7 +15456,7 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
@@ -15533,7 +15533,7 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G201" t="inlineStr">
@@ -15608,7 +15608,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
@@ -15683,7 +15683,7 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
@@ -15758,7 +15758,7 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
@@ -15833,7 +15833,7 @@
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
@@ -15908,7 +15908,7 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G206" t="inlineStr">
@@ -15983,7 +15983,7 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
@@ -16060,7 +16060,7 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
@@ -16135,7 +16135,7 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
@@ -16210,7 +16210,7 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G210" t="inlineStr">
@@ -16285,7 +16285,7 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G211" t="inlineStr">
@@ -16360,7 +16360,7 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
@@ -16437,7 +16437,7 @@
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G213" t="inlineStr">
@@ -16512,7 +16512,7 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
@@ -16587,7 +16587,7 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
@@ -16662,7 +16662,7 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
@@ -16737,7 +16737,7 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
@@ -16812,7 +16812,7 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
@@ -16887,7 +16887,7 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
@@ -16962,7 +16962,7 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
@@ -17037,7 +17037,7 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
@@ -17112,7 +17112,7 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
@@ -17187,7 +17187,7 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
@@ -17262,7 +17262,7 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
@@ -17337,7 +17337,7 @@
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
@@ -17412,7 +17412,7 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
@@ -17487,7 +17487,7 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
@@ -17562,7 +17562,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -17637,7 +17637,7 @@
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
@@ -17714,7 +17714,7 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
@@ -17789,7 +17789,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
@@ -17864,7 +17864,7 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
@@ -17939,7 +17939,7 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G233" t="inlineStr">
@@ -18014,7 +18014,7 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
@@ -18089,7 +18089,7 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
@@ -18166,7 +18166,7 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
@@ -18241,7 +18241,7 @@
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
@@ -18316,7 +18316,7 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
@@ -18391,7 +18391,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -18466,7 +18466,7 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G240" t="inlineStr">
@@ -18541,7 +18541,7 @@
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
@@ -18616,7 +18616,7 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
@@ -18691,7 +18691,7 @@
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
@@ -18766,7 +18766,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
@@ -18841,7 +18841,7 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G245" t="inlineStr">
@@ -18916,7 +18916,7 @@
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
@@ -18991,7 +18991,7 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
@@ -19066,7 +19066,7 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G248" t="inlineStr">
@@ -19141,7 +19141,7 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G249" t="inlineStr">
@@ -19216,7 +19216,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
@@ -19291,7 +19291,7 @@
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G251" t="inlineStr">
@@ -19366,7 +19366,7 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G252" t="inlineStr">
@@ -19443,7 +19443,7 @@
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G253" t="inlineStr">
@@ -19518,7 +19518,7 @@
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G254" t="inlineStr">
@@ -19593,7 +19593,7 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
@@ -19668,7 +19668,7 @@
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G256" t="inlineStr">
@@ -19743,7 +19743,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -19818,7 +19818,7 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G258" t="inlineStr">
@@ -19893,7 +19893,7 @@
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G259" t="inlineStr">
@@ -19968,7 +19968,7 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
@@ -20043,7 +20043,7 @@
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G261" t="inlineStr">
@@ -20118,7 +20118,7 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
@@ -20193,7 +20193,7 @@
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G263" t="inlineStr">
@@ -20268,7 +20268,7 @@
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G264" t="inlineStr">
@@ -20343,7 +20343,7 @@
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G265" t="inlineStr">
@@ -20418,7 +20418,7 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G266" t="inlineStr">
@@ -20493,7 +20493,7 @@
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
@@ -20568,7 +20568,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
@@ -20643,7 +20643,7 @@
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G269" t="inlineStr">
@@ -20718,7 +20718,7 @@
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G270" t="inlineStr">
@@ -20793,7 +20793,7 @@
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G271" t="inlineStr">
@@ -20870,7 +20870,7 @@
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G272" t="inlineStr">
@@ -20945,7 +20945,7 @@
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
@@ -21020,7 +21020,7 @@
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G274" t="inlineStr">
@@ -21095,7 +21095,7 @@
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G275" t="inlineStr">
@@ -21170,7 +21170,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
@@ -21245,7 +21245,7 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
@@ -21322,7 +21322,7 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
@@ -21397,7 +21397,7 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
@@ -21472,7 +21472,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
@@ -21547,7 +21547,7 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
@@ -21624,7 +21624,7 @@
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G282" t="inlineStr">
@@ -21699,7 +21699,7 @@
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
@@ -21776,7 +21776,7 @@
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G284" t="inlineStr">
@@ -21853,7 +21853,7 @@
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
@@ -21928,7 +21928,7 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
@@ -22003,7 +22003,7 @@
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
@@ -22078,7 +22078,7 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
@@ -22155,7 +22155,7 @@
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G289" t="inlineStr">
@@ -22230,7 +22230,7 @@
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
@@ -22305,7 +22305,7 @@
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
@@ -22380,7 +22380,7 @@
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
@@ -22455,7 +22455,7 @@
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G293" t="inlineStr">
@@ -22532,7 +22532,7 @@
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G294" t="inlineStr">
@@ -22607,7 +22607,7 @@
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
@@ -22682,7 +22682,7 @@
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
@@ -22757,7 +22757,7 @@
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
@@ -22832,7 +22832,7 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
@@ -22907,7 +22907,7 @@
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
@@ -22982,7 +22982,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
@@ -23057,7 +23057,7 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
@@ -23134,7 +23134,7 @@
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G302" t="inlineStr">
@@ -23209,7 +23209,7 @@
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
@@ -23284,7 +23284,7 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -23359,7 +23359,7 @@
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G305" t="inlineStr">
@@ -23436,7 +23436,7 @@
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G306" t="inlineStr">
@@ -23513,7 +23513,7 @@
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G307" t="inlineStr">
@@ -23590,7 +23590,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -23665,7 +23665,7 @@
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G309" t="inlineStr">
@@ -23740,7 +23740,7 @@
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G310" t="inlineStr">
@@ -23815,7 +23815,7 @@
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G311" t="inlineStr">
@@ -23890,7 +23890,7 @@
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G312" t="inlineStr">
@@ -23965,7 +23965,7 @@
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G313" t="inlineStr">
@@ -24042,7 +24042,7 @@
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G314" t="inlineStr">
@@ -24117,7 +24117,7 @@
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G315" t="inlineStr">
@@ -24192,7 +24192,7 @@
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G316" t="inlineStr">
@@ -24267,7 +24267,7 @@
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G317" t="inlineStr">
@@ -24342,7 +24342,7 @@
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G318" t="inlineStr">
@@ -24417,7 +24417,7 @@
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G319" t="inlineStr">
@@ -24492,7 +24492,7 @@
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G320" t="inlineStr">
@@ -24567,7 +24567,7 @@
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G321" t="inlineStr">
@@ -24642,7 +24642,7 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G322" t="inlineStr">
@@ -24717,7 +24717,7 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G323" t="inlineStr">
@@ -24792,7 +24792,7 @@
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G324" t="inlineStr">
@@ -24867,7 +24867,7 @@
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G325" t="inlineStr">
@@ -24942,7 +24942,7 @@
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G326" t="inlineStr">
@@ -25017,7 +25017,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G327" t="inlineStr">
@@ -25092,7 +25092,7 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G328" t="inlineStr">
@@ -25167,7 +25167,7 @@
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G329" t="inlineStr">
@@ -25242,7 +25242,7 @@
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G330" t="inlineStr">
@@ -25317,7 +25317,7 @@
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G331" t="inlineStr">
@@ -25392,7 +25392,7 @@
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G332" t="inlineStr">
@@ -25467,7 +25467,7 @@
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G333" t="inlineStr">
@@ -25542,7 +25542,7 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G334" t="inlineStr">
@@ -25617,7 +25617,7 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G335" t="inlineStr">
@@ -25692,7 +25692,7 @@
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G336" t="inlineStr">
@@ -25767,7 +25767,7 @@
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G337" t="inlineStr">
@@ -25844,7 +25844,7 @@
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G338" t="inlineStr">
@@ -25919,7 +25919,7 @@
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G339" t="inlineStr">
@@ -25994,7 +25994,7 @@
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G340" t="inlineStr">
@@ -26069,7 +26069,7 @@
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G341" t="inlineStr">
@@ -26144,7 +26144,7 @@
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G342" t="inlineStr">
@@ -26219,7 +26219,7 @@
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G343" t="inlineStr">
@@ -26294,7 +26294,7 @@
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G344" t="inlineStr">
@@ -26369,7 +26369,7 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G345" t="inlineStr">
@@ -26444,7 +26444,7 @@
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G346" t="inlineStr">
@@ -26521,7 +26521,7 @@
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G347" t="inlineStr">
@@ -26598,7 +26598,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G348" t="inlineStr">
@@ -26673,7 +26673,7 @@
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G349" t="inlineStr">
@@ -26750,7 +26750,7 @@
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G350" t="inlineStr">
@@ -26827,7 +26827,7 @@
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G351" t="inlineStr">
@@ -26902,7 +26902,7 @@
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G352" t="inlineStr">
@@ -26977,7 +26977,7 @@
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G353" t="inlineStr">
@@ -27052,7 +27052,7 @@
       </c>
       <c r="F354" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G354" t="inlineStr">
@@ -27127,7 +27127,7 @@
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G355" t="inlineStr">
@@ -27202,7 +27202,7 @@
       </c>
       <c r="F356" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G356" t="inlineStr">
@@ -27277,7 +27277,7 @@
       </c>
       <c r="F357" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G357" t="inlineStr">
@@ -27352,7 +27352,7 @@
       </c>
       <c r="F358" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G358" t="inlineStr">
@@ -27427,7 +27427,7 @@
       </c>
       <c r="F359" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G359" t="inlineStr">
@@ -27502,7 +27502,7 @@
       </c>
       <c r="F360" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G360" t="inlineStr">
@@ -27577,7 +27577,7 @@
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G361" t="inlineStr">
@@ -27652,7 +27652,7 @@
       </c>
       <c r="F362" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G362" t="inlineStr">
@@ -27727,7 +27727,7 @@
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G363" t="inlineStr">
@@ -27802,7 +27802,7 @@
       </c>
       <c r="F364" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G364" t="inlineStr">
@@ -27879,7 +27879,7 @@
       </c>
       <c r="F365" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G365" t="inlineStr">
@@ -27954,7 +27954,7 @@
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G366" t="inlineStr">
@@ -28029,7 +28029,7 @@
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G367" t="inlineStr">
@@ -28104,7 +28104,7 @@
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G368" t="inlineStr">
@@ -28181,7 +28181,7 @@
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G369" t="inlineStr">
@@ -28256,7 +28256,7 @@
       </c>
       <c r="F370" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G370" t="inlineStr">
@@ -28331,7 +28331,7 @@
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G371" t="inlineStr">
@@ -28406,7 +28406,7 @@
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G372" t="inlineStr">
@@ -28481,7 +28481,7 @@
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G373" t="inlineStr">
@@ -28556,7 +28556,7 @@
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G374" t="inlineStr">
@@ -28631,7 +28631,7 @@
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G375" t="inlineStr">
@@ -28706,7 +28706,7 @@
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G376" t="inlineStr">
@@ -28781,7 +28781,7 @@
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G377" t="inlineStr">
@@ -28856,7 +28856,7 @@
       </c>
       <c r="F378" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G378" t="inlineStr">
@@ -28931,7 +28931,7 @@
       </c>
       <c r="F379" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G379" t="inlineStr">
@@ -29006,7 +29006,7 @@
       </c>
       <c r="F380" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G380" t="inlineStr">
@@ -29081,7 +29081,7 @@
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G381" t="inlineStr">
@@ -29156,7 +29156,7 @@
       </c>
       <c r="F382" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G382" t="inlineStr">
@@ -29231,7 +29231,7 @@
       </c>
       <c r="F383" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G383" t="inlineStr">
@@ -29308,7 +29308,7 @@
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G384" t="inlineStr">
@@ -29383,7 +29383,7 @@
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G385" t="inlineStr">
@@ -29458,7 +29458,7 @@
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G386" t="inlineStr">
@@ -29533,7 +29533,7 @@
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G387" t="inlineStr">
@@ -29608,7 +29608,7 @@
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G388" t="inlineStr">
@@ -29683,7 +29683,7 @@
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G389" t="inlineStr">
@@ -29760,7 +29760,7 @@
       </c>
       <c r="F390" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G390" t="inlineStr">
@@ -29837,7 +29837,7 @@
       </c>
       <c r="F391" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G391" t="inlineStr">
@@ -29912,7 +29912,7 @@
       </c>
       <c r="F392" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G392" t="inlineStr">
@@ -29989,7 +29989,7 @@
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G393" t="inlineStr">
@@ -30064,7 +30064,7 @@
       </c>
       <c r="F394" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G394" t="inlineStr">
@@ -30139,7 +30139,7 @@
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G395" t="inlineStr">
@@ -30214,7 +30214,7 @@
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G396" t="inlineStr">
@@ -30289,7 +30289,7 @@
       </c>
       <c r="F397" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G397" t="inlineStr">
@@ -30364,7 +30364,7 @@
       </c>
       <c r="F398" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G398" t="inlineStr">
@@ -30439,7 +30439,7 @@
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G399" t="inlineStr">
@@ -30514,7 +30514,7 @@
       </c>
       <c r="F400" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G400" t="inlineStr">
@@ -30589,7 +30589,7 @@
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G401" t="inlineStr">
@@ -30664,7 +30664,7 @@
       </c>
       <c r="F402" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G402" t="inlineStr">
@@ -30739,7 +30739,7 @@
       </c>
       <c r="F403" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G403" t="inlineStr">
@@ -30814,7 +30814,7 @@
       </c>
       <c r="F404" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G404" t="inlineStr">
@@ -30891,7 +30891,7 @@
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G405" t="inlineStr">
@@ -30966,7 +30966,7 @@
       </c>
       <c r="F406" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G406" t="inlineStr">
@@ -31041,7 +31041,7 @@
       </c>
       <c r="F407" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G407" t="inlineStr">
@@ -31116,7 +31116,7 @@
       </c>
       <c r="F408" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G408" t="inlineStr">
@@ -31191,7 +31191,7 @@
       </c>
       <c r="F409" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G409" t="inlineStr">
@@ -31266,7 +31266,7 @@
       </c>
       <c r="F410" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G410" t="inlineStr">
@@ -31341,7 +31341,7 @@
       </c>
       <c r="F411" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G411" t="inlineStr">
@@ -31416,7 +31416,7 @@
       </c>
       <c r="F412" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G412" t="inlineStr">
@@ -31491,7 +31491,7 @@
       </c>
       <c r="F413" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G413" t="inlineStr">
@@ -31566,7 +31566,7 @@
       </c>
       <c r="F414" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G414" t="inlineStr">
@@ -31641,7 +31641,7 @@
       </c>
       <c r="F415" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G415" t="inlineStr">
@@ -31716,7 +31716,7 @@
       </c>
       <c r="F416" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G416" t="inlineStr">
@@ -31791,7 +31791,7 @@
       </c>
       <c r="F417" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G417" t="inlineStr">
@@ -31866,7 +31866,7 @@
       </c>
       <c r="F418" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G418" t="inlineStr">
@@ -31943,7 +31943,7 @@
       </c>
       <c r="F419" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G419" t="inlineStr">
@@ -32018,7 +32018,7 @@
       </c>
       <c r="F420" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G420" t="inlineStr">
@@ -32093,7 +32093,7 @@
       </c>
       <c r="F421" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G421" t="inlineStr">
@@ -32168,7 +32168,7 @@
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G422" t="inlineStr">
@@ -32243,7 +32243,7 @@
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G423" t="inlineStr">
@@ -32318,7 +32318,7 @@
       </c>
       <c r="F424" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G424" t="inlineStr">
@@ -32393,7 +32393,7 @@
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G425" t="inlineStr">
@@ -32468,7 +32468,7 @@
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G426" t="inlineStr">
@@ -32543,7 +32543,7 @@
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>Financing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G427" t="inlineStr">
@@ -32618,7 +32618,7 @@
       </c>
       <c r="F428" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G428" t="inlineStr">
@@ -32693,7 +32693,7 @@
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G429" t="inlineStr">
@@ -32770,7 +32770,7 @@
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G430" t="inlineStr">
@@ -32845,7 +32845,7 @@
       </c>
       <c r="F431" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G431" t="inlineStr">
@@ -32920,7 +32920,7 @@
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G432" t="inlineStr">
@@ -32995,7 +32995,7 @@
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G433" t="inlineStr">
@@ -33070,7 +33070,7 @@
       </c>
       <c r="F434" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G434" t="inlineStr">
@@ -33145,7 +33145,7 @@
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G435" t="inlineStr">
@@ -33220,7 +33220,7 @@
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G436" t="inlineStr">
@@ -33297,7 +33297,7 @@
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G437" t="inlineStr">
@@ -33372,7 +33372,7 @@
       </c>
       <c r="F438" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G438" t="inlineStr">
@@ -33447,7 +33447,7 @@
       </c>
       <c r="F439" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G439" t="inlineStr">
@@ -33524,7 +33524,7 @@
       </c>
       <c r="F440" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G440" t="inlineStr">
@@ -33601,7 +33601,7 @@
       </c>
       <c r="F441" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G441" t="inlineStr">
@@ -33676,7 +33676,7 @@
       </c>
       <c r="F442" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G442" t="inlineStr">
@@ -33751,7 +33751,7 @@
       </c>
       <c r="F443" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G443" t="inlineStr">
@@ -33826,7 +33826,7 @@
       </c>
       <c r="F444" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G444" t="inlineStr">
@@ -33903,7 +33903,7 @@
       </c>
       <c r="F445" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G445" t="inlineStr">
@@ -33978,7 +33978,7 @@
       </c>
       <c r="F446" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G446" t="inlineStr">
@@ -34053,7 +34053,7 @@
       </c>
       <c r="F447" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G447" t="inlineStr">
@@ -34128,7 +34128,7 @@
       </c>
       <c r="F448" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G448" t="inlineStr">
@@ -34203,7 +34203,7 @@
       </c>
       <c r="F449" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G449" t="inlineStr">
@@ -34278,7 +34278,7 @@
       </c>
       <c r="F450" t="inlineStr">
         <is>
-          <t>Investing Activities (ML)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G450" t="inlineStr">
@@ -34353,7 +34353,7 @@
       </c>
       <c r="F451" t="inlineStr">
         <is>
-          <t>Operating Activities (ML)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G451" t="inlineStr">

</xml_diff>

<commit_message>
done with 5 parameters ollama + xgboost
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -625,7 +625,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2883,7 +2883,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -3183,7 +3183,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -3939,7 +3939,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -4239,7 +4239,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -4764,7 +4764,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -4916,7 +4916,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -5291,7 +5291,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -5441,7 +5441,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -6193,7 +6193,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -6495,7 +6495,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -6874,7 +6874,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -6951,7 +6951,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -7251,7 +7251,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -7326,7 +7326,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -8228,7 +8228,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -8303,7 +8303,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -8455,7 +8455,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -8757,7 +8757,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -9057,7 +9057,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -9207,7 +9207,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -9359,7 +9359,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -9586,7 +9586,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -9890,7 +9890,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -10040,7 +10040,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
@@ -10190,7 +10190,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -10417,7 +10417,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -10492,7 +10492,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -10569,7 +10569,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -11171,7 +11171,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
@@ -11246,7 +11246,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -11321,7 +11321,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -11471,7 +11471,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -12071,7 +12071,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
@@ -12225,7 +12225,7 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
@@ -12450,7 +12450,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
@@ -12600,7 +12600,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
@@ -13200,7 +13200,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
@@ -13275,7 +13275,7 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
@@ -13654,7 +13654,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
@@ -13804,7 +13804,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
@@ -13954,7 +13954,7 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
@@ -14329,7 +14329,7 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
@@ -14629,7 +14629,7 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
@@ -14929,7 +14929,7 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
@@ -15004,7 +15004,7 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
@@ -15456,7 +15456,7 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
@@ -15908,7 +15908,7 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G206" t="inlineStr">
@@ -15983,7 +15983,7 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
@@ -16662,7 +16662,7 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
@@ -16737,7 +16737,7 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
@@ -17187,7 +17187,7 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
@@ -17262,7 +17262,7 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
@@ -17562,7 +17562,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -18391,7 +18391,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -18541,7 +18541,7 @@
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
@@ -18916,7 +18916,7 @@
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
@@ -18991,7 +18991,7 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
@@ -19141,7 +19141,7 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G249" t="inlineStr">
@@ -19743,7 +19743,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -19818,7 +19818,7 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G258" t="inlineStr">
@@ -19893,7 +19893,7 @@
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G259" t="inlineStr">
@@ -20118,7 +20118,7 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
@@ -20343,7 +20343,7 @@
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G265" t="inlineStr">
@@ -20418,7 +20418,7 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G266" t="inlineStr">
@@ -20493,7 +20493,7 @@
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
@@ -20568,7 +20568,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
@@ -20945,7 +20945,7 @@
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
@@ -21170,7 +21170,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
@@ -21624,7 +21624,7 @@
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G282" t="inlineStr">
@@ -22003,7 +22003,7 @@
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
@@ -22380,7 +22380,7 @@
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
@@ -22532,7 +22532,7 @@
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G294" t="inlineStr">
@@ -22607,7 +22607,7 @@
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
@@ -22832,7 +22832,7 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
@@ -22907,7 +22907,7 @@
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
@@ -22982,7 +22982,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
@@ -23057,7 +23057,7 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
@@ -23284,7 +23284,7 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -24417,7 +24417,7 @@
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G319" t="inlineStr">
@@ -24492,7 +24492,7 @@
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G320" t="inlineStr">
@@ -25017,7 +25017,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G327" t="inlineStr">
@@ -25092,7 +25092,7 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G328" t="inlineStr">
@@ -25242,7 +25242,7 @@
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G330" t="inlineStr">
@@ -25919,7 +25919,7 @@
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G339" t="inlineStr">
@@ -27052,7 +27052,7 @@
       </c>
       <c r="F354" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G354" t="inlineStr">
@@ -28181,7 +28181,7 @@
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G369" t="inlineStr">
@@ -28631,7 +28631,7 @@
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G375" t="inlineStr">
@@ -28781,7 +28781,7 @@
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G377" t="inlineStr">
@@ -28931,7 +28931,7 @@
       </c>
       <c r="F379" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G379" t="inlineStr">
@@ -29383,7 +29383,7 @@
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G385" t="inlineStr">
@@ -29458,7 +29458,7 @@
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G386" t="inlineStr">
@@ -29912,7 +29912,7 @@
       </c>
       <c r="F392" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G392" t="inlineStr">
@@ -30439,7 +30439,7 @@
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G399" t="inlineStr">
@@ -30514,7 +30514,7 @@
       </c>
       <c r="F400" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G400" t="inlineStr">
@@ -30739,7 +30739,7 @@
       </c>
       <c r="F403" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G403" t="inlineStr">
@@ -30814,7 +30814,7 @@
       </c>
       <c r="F404" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G404" t="inlineStr">
@@ -30891,7 +30891,7 @@
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G405" t="inlineStr">
@@ -31116,7 +31116,7 @@
       </c>
       <c r="F408" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G408" t="inlineStr">
@@ -31341,7 +31341,7 @@
       </c>
       <c r="F411" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G411" t="inlineStr">
@@ -31416,7 +31416,7 @@
       </c>
       <c r="F412" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G412" t="inlineStr">
@@ -31641,7 +31641,7 @@
       </c>
       <c r="F415" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G415" t="inlineStr">
@@ -31943,7 +31943,7 @@
       </c>
       <c r="F419" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G419" t="inlineStr">
@@ -32770,7 +32770,7 @@
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G430" t="inlineStr">
@@ -32995,7 +32995,7 @@
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G433" t="inlineStr">
@@ -33070,7 +33070,7 @@
       </c>
       <c r="F434" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G434" t="inlineStr">
@@ -33145,7 +33145,7 @@
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G435" t="inlineStr">
@@ -33297,7 +33297,7 @@
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G437" t="inlineStr">
@@ -33372,7 +33372,7 @@
       </c>
       <c r="F438" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G438" t="inlineStr">
@@ -33676,7 +33676,7 @@
       </c>
       <c r="F442" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G442" t="inlineStr">
@@ -33978,7 +33978,7 @@
       </c>
       <c r="F446" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G446" t="inlineStr">
@@ -34053,7 +34053,7 @@
       </c>
       <c r="F447" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G447" t="inlineStr">
@@ -34203,7 +34203,7 @@
       </c>
       <c r="F449" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G449" t="inlineStr">
@@ -34278,7 +34278,7 @@
       </c>
       <c r="F450" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G450" t="inlineStr">

</xml_diff>

<commit_message>
14 paramerters with full ai and xgboost
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -700,7 +700,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1227,7 +1227,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1377,7 +1377,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -3183,7 +3183,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -3333,7 +3333,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -3939,7 +3939,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -5066,7 +5066,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -5591,7 +5591,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -5966,7 +5966,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -6041,7 +6041,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -6118,7 +6118,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -6724,7 +6724,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -6874,7 +6874,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -6951,7 +6951,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -7026,7 +7026,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -7251,7 +7251,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -7851,7 +7851,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -8228,7 +8228,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -8455,7 +8455,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -8605,7 +8605,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -8682,7 +8682,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -8982,7 +8982,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -9815,7 +9815,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
@@ -11846,7 +11846,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -11996,7 +11996,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
@@ -12900,7 +12900,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
@@ -12975,7 +12975,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
@@ -13200,7 +13200,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
@@ -13579,7 +13579,7 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
@@ -13654,7 +13654,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
@@ -13804,7 +13804,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
@@ -15683,7 +15683,7 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
@@ -16060,7 +16060,7 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
@@ -16135,7 +16135,7 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
@@ -16285,7 +16285,7 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G211" t="inlineStr">
@@ -16887,7 +16887,7 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
@@ -17187,7 +17187,7 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
@@ -17262,7 +17262,7 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
@@ -17562,7 +17562,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -18014,7 +18014,7 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
@@ -18241,7 +18241,7 @@
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
@@ -18766,7 +18766,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
@@ -19593,7 +19593,7 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
@@ -19818,7 +19818,7 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G258" t="inlineStr">
@@ -20043,7 +20043,7 @@
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G261" t="inlineStr">
@@ -20343,7 +20343,7 @@
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G265" t="inlineStr">
@@ -20568,7 +20568,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
@@ -21020,7 +21020,7 @@
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G274" t="inlineStr">
@@ -21095,7 +21095,7 @@
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G275" t="inlineStr">
@@ -21170,7 +21170,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
@@ -21624,7 +21624,7 @@
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G282" t="inlineStr">
@@ -21853,7 +21853,7 @@
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
@@ -22455,7 +22455,7 @@
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G293" t="inlineStr">
@@ -22607,7 +22607,7 @@
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
@@ -22832,7 +22832,7 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
@@ -22982,7 +22982,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
@@ -23057,7 +23057,7 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
@@ -23209,7 +23209,7 @@
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
@@ -23284,7 +23284,7 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -23590,7 +23590,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -23665,7 +23665,7 @@
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G309" t="inlineStr">
@@ -23890,7 +23890,7 @@
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G312" t="inlineStr">
@@ -24267,7 +24267,7 @@
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G317" t="inlineStr">
@@ -24492,7 +24492,7 @@
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G320" t="inlineStr">
@@ -25017,7 +25017,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G327" t="inlineStr">
@@ -25467,7 +25467,7 @@
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G333" t="inlineStr">
@@ -25692,7 +25692,7 @@
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G336" t="inlineStr">
@@ -26598,7 +26598,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G348" t="inlineStr">
@@ -26827,7 +26827,7 @@
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G351" t="inlineStr">
@@ -27127,7 +27127,7 @@
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G355" t="inlineStr">
@@ -27427,7 +27427,7 @@
       </c>
       <c r="F359" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G359" t="inlineStr">
@@ -27727,7 +27727,7 @@
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G363" t="inlineStr">
@@ -27954,7 +27954,7 @@
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G366" t="inlineStr">
@@ -28181,7 +28181,7 @@
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G369" t="inlineStr">
@@ -28331,7 +28331,7 @@
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G371" t="inlineStr">
@@ -28631,7 +28631,7 @@
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G375" t="inlineStr">
@@ -29308,7 +29308,7 @@
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G384" t="inlineStr">
@@ -29383,7 +29383,7 @@
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G385" t="inlineStr">
@@ -29458,7 +29458,7 @@
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G386" t="inlineStr">
@@ -29989,7 +29989,7 @@
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G393" t="inlineStr">
@@ -30214,7 +30214,7 @@
       </c>
       <c r="F396" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G396" t="inlineStr">
@@ -30589,7 +30589,7 @@
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G401" t="inlineStr">
@@ -31116,7 +31116,7 @@
       </c>
       <c r="F408" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G408" t="inlineStr">
@@ -31416,7 +31416,7 @@
       </c>
       <c r="F412" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G412" t="inlineStr">
@@ -31641,7 +31641,7 @@
       </c>
       <c r="F415" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G415" t="inlineStr">
@@ -32018,7 +32018,7 @@
       </c>
       <c r="F420" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G420" t="inlineStr">
@@ -32168,7 +32168,7 @@
       </c>
       <c r="F422" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G422" t="inlineStr">
@@ -32243,7 +32243,7 @@
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G423" t="inlineStr">
@@ -32468,7 +32468,7 @@
       </c>
       <c r="F426" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G426" t="inlineStr">
@@ -32693,7 +32693,7 @@
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G429" t="inlineStr">
@@ -32770,7 +32770,7 @@
       </c>
       <c r="F430" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G430" t="inlineStr">
@@ -32920,7 +32920,7 @@
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G432" t="inlineStr">
@@ -32995,7 +32995,7 @@
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G433" t="inlineStr">
@@ -33145,7 +33145,7 @@
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G435" t="inlineStr">
@@ -33676,7 +33676,7 @@
       </c>
       <c r="F442" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G442" t="inlineStr">
@@ -34053,7 +34053,7 @@
       </c>
       <c r="F447" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G447" t="inlineStr">
@@ -34128,7 +34128,7 @@
       </c>
       <c r="F448" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G448" t="inlineStr">

</xml_diff>

<commit_message>
categories nothing to change
</commit_message>
<xml_diff>
--- a/data/bank_data_processed.xlsx
+++ b/data/bank_data_processed.xlsx
@@ -2958,7 +2958,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -10417,7 +10417,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -11096,7 +11096,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -11321,7 +11321,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -13275,7 +13275,7 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
@@ -15004,7 +15004,7 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
@@ -15533,7 +15533,7 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G201" t="inlineStr">
@@ -16737,7 +16737,7 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
@@ -17112,7 +17112,7 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
@@ -19443,7 +19443,7 @@
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G253" t="inlineStr">
@@ -22682,7 +22682,7 @@
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
@@ -23284,7 +23284,7 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -23590,7 +23590,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -25242,7 +25242,7 @@
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G330" t="inlineStr">
@@ -26219,7 +26219,7 @@
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G343" t="inlineStr">
@@ -26598,7 +26598,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Financing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G348" t="inlineStr">
@@ -28181,7 +28181,7 @@
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>Financing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G369" t="inlineStr">
@@ -30589,7 +30589,7 @@
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G401" t="inlineStr">
@@ -31566,7 +31566,7 @@
       </c>
       <c r="F414" t="inlineStr">
         <is>
-          <t>Investing Activities (XGBoost)</t>
+          <t>Operating Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G414" t="inlineStr">
@@ -34128,7 +34128,7 @@
       </c>
       <c r="F448" t="inlineStr">
         <is>
-          <t>Operating Activities (XGBoost)</t>
+          <t>Investing Activities (XGBoost)</t>
         </is>
       </c>
       <c r="G448" t="inlineStr">

</xml_diff>